<commit_message>
Analysis FreqDoubling Variable Attenuator
</commit_message>
<xml_diff>
--- a/245/data/Super_awesome_optical_freq_doubling.xlsx
+++ b/245/data/Super_awesome_optical_freq_doubling.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="19035" windowHeight="8445" activeTab="6"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="19035" windowHeight="8445" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="139">
   <si>
     <t>Error</t>
   </si>
@@ -246,17 +246,210 @@
   </si>
   <si>
     <t>lamba</t>
+  </si>
+  <si>
+    <t>118.0 \pm 1.0</t>
+  </si>
+  <si>
+    <t>115.0 \pm 1.0</t>
+  </si>
+  <si>
+    <t>113.0 \pm 1.0</t>
+  </si>
+  <si>
+    <t>107.0 \pm 1.0</t>
+  </si>
+  <si>
+    <t>101.0 \pm 1.0</t>
+  </si>
+  <si>
+    <t>94.0 \pm 1.0</t>
+  </si>
+  <si>
+    <t>85.0 \pm 1.0</t>
+  </si>
+  <si>
+    <t>75.0 \pm 1.0</t>
+  </si>
+  <si>
+    <t>65.0 \pm 1.0</t>
+  </si>
+  <si>
+    <t>55.0 \pm 1.0</t>
+  </si>
+  <si>
+    <t>46.0 \pm 1.0</t>
+  </si>
+  <si>
+    <t>36.0 \pm 1.0</t>
+  </si>
+  <si>
+    <t>26.0 \pm 1.0</t>
+  </si>
+  <si>
+    <t>20.0 \pm 1.0</t>
+  </si>
+  <si>
+    <t>13.0 \pm 1.0</t>
+  </si>
+  <si>
+    <t>7.0 \pm 0.1</t>
+  </si>
+  <si>
+    <t>3.0 \pm 0.1</t>
+  </si>
+  <si>
+    <t>0.8 \pm 0.1</t>
+  </si>
+  <si>
+    <t>0.3 \pm 0.1</t>
+  </si>
+  <si>
+    <t>1.5 \pm 0.1</t>
+  </si>
+  <si>
+    <t>4.8 \pm 0.1</t>
+  </si>
+  <si>
+    <t>8.8 \pm 0.1</t>
+  </si>
+  <si>
+    <t>16.0 \pm 1.0</t>
+  </si>
+  <si>
+    <t>23.0 \pm 1.0</t>
+  </si>
+  <si>
+    <t>32.0 \pm 1.0</t>
+  </si>
+  <si>
+    <t>41.0 \pm 1.0</t>
+  </si>
+  <si>
+    <t>51.0 \pm 1.0</t>
+  </si>
+  <si>
+    <t>61.0 \pm 1.0</t>
+  </si>
+  <si>
+    <t>72.0 \pm 1.0</t>
+  </si>
+  <si>
+    <t>80.0 \pm 1.0</t>
+  </si>
+  <si>
+    <t>90.0 \pm 1.0</t>
+  </si>
+  <si>
+    <t>97.0 \pm 1.0</t>
+  </si>
+  <si>
+    <t>105.0 \pm 1.0</t>
+  </si>
+  <si>
+    <t>110.0 \pm 1.0</t>
+  </si>
+  <si>
+    <t>117.0 \pm 1.0</t>
+  </si>
+  <si>
+    <t>116.0 \pm 1.0</t>
+  </si>
+  <si>
+    <t>109.0 \pm 1.0</t>
+  </si>
+  <si>
+    <t>102.0 \pm 1.0</t>
+  </si>
+  <si>
+    <t>95.0 \pm 1.0</t>
+  </si>
+  <si>
+    <t>87.0 \pm 1.0</t>
+  </si>
+  <si>
+    <t>78.0 \pm 1.0</t>
+  </si>
+  <si>
+    <t>67.0 \pm 1.0</t>
+  </si>
+  <si>
+    <t>58.0 \pm 1.0</t>
+  </si>
+  <si>
+    <t>39.0 \pm 1.0</t>
+  </si>
+  <si>
+    <t>28.0 \pm 1.0</t>
+  </si>
+  <si>
+    <t>21.0 \pm 1.0</t>
+  </si>
+  <si>
+    <t>8.0 \pm 0.1</t>
+  </si>
+  <si>
+    <t>4.0 \pm 0.1</t>
+  </si>
+  <si>
+    <t>2.0 \pm 0.1</t>
+  </si>
+  <si>
+    <t>1.9 \pm 0.1</t>
+  </si>
+  <si>
+    <t>5.0 \pm 0.1</t>
+  </si>
+  <si>
+    <t>9.0 \pm 0.1</t>
+  </si>
+  <si>
+    <t>22.0 \pm 1.0</t>
+  </si>
+  <si>
+    <t>31.0 \pm 1.0</t>
+  </si>
+  <si>
+    <t>40.0 \pm 1.0</t>
+  </si>
+  <si>
+    <t>50.0 \pm 1.0</t>
+  </si>
+  <si>
+    <t>60.0 \pm 1.0</t>
+  </si>
+  <si>
+    <t>71.0 \pm 1.0</t>
+  </si>
+  <si>
+    <t>106.0 \pm 1.0</t>
+  </si>
+  <si>
+    <t>111.0 \pm 1.0</t>
+  </si>
+  <si>
+    <t>96.0 \pm 1.0</t>
+  </si>
+  <si>
+    <t>86.0 \pm 1.0</t>
+  </si>
+  <si>
+    <t>1.0 \pm 0.1</t>
+  </si>
+  <si>
+    <t>0.4 \pm 0.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
     <numFmt numFmtId="166" formatCode="0.0E+00"/>
     <numFmt numFmtId="167" formatCode="0.0000000000"/>
+    <numFmt numFmtId="168" formatCode="0.0"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -324,7 +517,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -338,6 +531,7 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -677,8 +871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1044,12 +1238,12 @@
         <v>0.1</v>
       </c>
       <c r="I20">
-        <f>J14*1000/O14</f>
-        <v>975.98694826498524</v>
+        <f>J14*1000/J8</f>
+        <v>1048.9021503839599</v>
       </c>
       <c r="J20">
-        <f>SQRT((K14*1000/(O14))^2 + (J14*P14/(O14^2))^2)</f>
-        <v>33.521301917329254</v>
+        <f>SQRT((K14*1000/(J8))^2 + (J14*K8/(J8^2))^2)</f>
+        <v>36.02564173527626</v>
       </c>
     </row>
     <row r="21" spans="1:16">
@@ -1139,7 +1333,7 @@
       </c>
       <c r="O25">
         <f>SQRT((K28/J27)^2+(J28*K27/(J27^2))^2)</f>
-        <v>2.8839745780208048</v>
+        <v>2.8839738080437609</v>
       </c>
       <c r="P25" t="s">
         <v>48</v>
@@ -1169,11 +1363,11 @@
       </c>
       <c r="N26">
         <f>J27*0.000796069256545841</f>
-        <v>0.4457831165949116</v>
+        <v>0.47908721569739188</v>
       </c>
       <c r="O26">
         <f>K27*0.000796069256545841</f>
-        <v>1.5422151423301162E-2</v>
+        <v>1.6574323559919987E-2</v>
       </c>
     </row>
     <row r="27" spans="1:16">
@@ -1194,11 +1388,11 @@
       </c>
       <c r="J27">
         <f>J8*I20</f>
-        <v>559.98031946262142</v>
+        <v>601.81600000000003</v>
       </c>
       <c r="K27">
         <f>SQRT((K8*I20)^2+(J8*J20)^2)</f>
-        <v>19.372876538679758</v>
+        <v>20.820203045946375</v>
       </c>
       <c r="L27" t="s">
         <v>39</v>
@@ -1222,11 +1416,11 @@
       </c>
       <c r="J28">
         <f>J9*I20</f>
-        <v>-33001.72987254773</v>
+        <v>-35467.262642438101</v>
       </c>
       <c r="K28">
         <f>SQRT((K9*I20)^2+(J9*J20)^2)</f>
-        <v>1142.1951130658861</v>
+        <v>1227.5272662770337</v>
       </c>
       <c r="L28" t="s">
         <v>40</v>
@@ -1553,8 +1747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K98"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1563,6 +1757,7 @@
     <col min="3" max="3" width="21" customWidth="1"/>
     <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="8" max="8" width="16.5703125" customWidth="1"/>
+    <col min="9" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="14.25" customHeight="1">
@@ -1626,11 +1821,11 @@
       </c>
       <c r="E8">
         <f>C8*$H$18</f>
-        <v>115.16645989526825</v>
+        <v>123.77045374530726</v>
       </c>
       <c r="F8">
         <f>SQRT((D8*$H$18)^2+(C8*$I$18)^2)</f>
-        <v>4.0741426792139102</v>
+        <v>1.04890215038396</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1648,11 +1843,11 @@
       </c>
       <c r="E9">
         <f t="shared" ref="E9:E72" si="0">C9*$H$18</f>
-        <v>112.23849905047331</v>
+        <v>120.62374729415539</v>
       </c>
       <c r="F9">
         <f t="shared" ref="F9:F72" si="1">SQRT((D9*$H$18)^2+(C9*$I$18)^2)</f>
-        <v>3.9765799213283279</v>
+        <v>1.04890215038396</v>
       </c>
       <c r="I9" s="8" t="s">
         <v>34</v>
@@ -1676,20 +1871,22 @@
       </c>
       <c r="E10">
         <f t="shared" si="0"/>
-        <v>110.28652515394333</v>
+        <v>118.52594299338747</v>
       </c>
       <c r="F10">
         <f t="shared" si="1"/>
-        <v>3.9116225338871184</v>
+        <v>1.04890215038396</v>
       </c>
       <c r="H10" t="s">
         <v>51</v>
       </c>
       <c r="I10" s="3">
-        <v>112.553</v>
+        <f>117.861*H18/1000</f>
+        <v>123.62465634640391</v>
       </c>
       <c r="J10" s="3">
-        <v>0.37819999999999998</v>
+        <f>SQRT((0.6052*H18/1000)^2+(J18*117.861/1000)^2)</f>
+        <v>4.2932080837059239</v>
       </c>
       <c r="K10" t="s">
         <v>42</v>
@@ -1710,20 +1907,20 @@
       </c>
       <c r="E11">
         <f t="shared" si="0"/>
-        <v>104.43060346435342</v>
+        <v>112.2325300910837</v>
       </c>
       <c r="F11">
         <f t="shared" si="1"/>
-        <v>3.7171946824273627</v>
+        <v>1.04890215038396</v>
       </c>
       <c r="H11" t="s">
         <v>36</v>
       </c>
       <c r="I11" s="7">
-        <v>2.0047392181170904</v>
+        <v>2.00285</v>
       </c>
       <c r="J11" s="7">
-        <v>7.5802316295807892E-4</v>
+        <v>8.9240000000000001E-4</v>
       </c>
       <c r="K11" t="s">
         <v>54</v>
@@ -1744,11 +1941,11 @@
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
-        <v>98.574681774763519</v>
+        <v>105.93911718877996</v>
       </c>
       <c r="F12">
         <f t="shared" si="1"/>
-        <v>3.523519059071456</v>
+        <v>1.04890215038396</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1766,11 +1963,11 @@
       </c>
       <c r="E13">
         <f t="shared" si="0"/>
-        <v>91.74277313690861</v>
+        <v>98.596802136092236</v>
       </c>
       <c r="F13">
         <f t="shared" si="1"/>
-        <v>3.2986916381183775</v>
+        <v>1.04890215038396</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -1788,11 +1985,11 @@
       </c>
       <c r="E14">
         <f t="shared" si="0"/>
-        <v>82.958890602523752</v>
+        <v>89.156682782636594</v>
       </c>
       <c r="F14">
         <f t="shared" si="1"/>
-        <v>3.0118303035388894</v>
+        <v>1.04890215038396</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1810,11 +2007,11 @@
       </c>
       <c r="E15">
         <f t="shared" si="0"/>
-        <v>73.19902111987389</v>
+        <v>78.667661278796984</v>
       </c>
       <c r="F15">
         <f t="shared" si="1"/>
-        <v>2.6968940442187885</v>
+        <v>1.04890215038396</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1832,11 +2029,11 @@
       </c>
       <c r="E16">
         <f t="shared" si="0"/>
-        <v>63.439151637224043</v>
+        <v>68.178639774957389</v>
       </c>
       <c r="F16">
         <f t="shared" si="1"/>
-        <v>2.3874858597731916</v>
+        <v>1.04890215038396</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>52</v>
@@ -1858,16 +2055,19 @@
       </c>
       <c r="E17">
         <f t="shared" si="0"/>
-        <v>53.679282154574189</v>
+        <v>57.689618271117794</v>
       </c>
       <c r="F17">
         <f t="shared" si="1"/>
-        <v>2.0860669960328799</v>
+        <v>1.04890215038396</v>
       </c>
       <c r="H17" s="8" t="s">
         <v>34</v>
       </c>
       <c r="I17" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J17" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1886,17 +2086,22 @@
       </c>
       <c r="E18">
         <f t="shared" si="0"/>
-        <v>44.895399620189323</v>
+        <v>48.249498917662152</v>
       </c>
       <c r="F18">
         <f t="shared" si="1"/>
-        <v>1.8248979420197944</v>
+        <v>1.04890215038396</v>
       </c>
       <c r="H18" s="6">
-        <v>975.98694826498524</v>
+        <v>1048.9021503839599</v>
       </c>
       <c r="I18">
-        <v>33.521301917329254</v>
+        <f>36.0256417352763*0</f>
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <f>36.0256417352763</f>
+        <v>36.025641735276302</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -1914,11 +2119,11 @@
       </c>
       <c r="E19">
         <f t="shared" si="0"/>
-        <v>35.135530137539469</v>
+        <v>37.760477413822557</v>
       </c>
       <c r="F19">
         <f t="shared" si="1"/>
-        <v>1.5520427827083996</v>
+        <v>1.04890215038396</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1936,11 +2141,11 @@
       </c>
       <c r="E20">
         <f t="shared" si="0"/>
-        <v>25.375660654889614</v>
+        <v>27.271455909982958</v>
       </c>
       <c r="F20">
         <f t="shared" si="1"/>
-        <v>1.3084940337551916</v>
+        <v>1.04890215038396</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1958,11 +2163,11 @@
       </c>
       <c r="E21">
         <f t="shared" si="0"/>
-        <v>19.519738965299705</v>
+        <v>20.978043007679197</v>
       </c>
       <c r="F21">
         <f t="shared" si="1"/>
-        <v>1.1840699287105876</v>
+        <v>1.04890215038396</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1980,11 +2185,11 @@
       </c>
       <c r="E22">
         <f t="shared" si="0"/>
-        <v>12.687830327444807</v>
+        <v>13.635727954991479</v>
       </c>
       <c r="F22">
         <f t="shared" si="1"/>
-        <v>1.0688554867150808</v>
+        <v>1.04890215038396</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -2002,11 +2207,11 @@
       </c>
       <c r="E23">
         <f t="shared" si="0"/>
-        <v>6.8319086378548972</v>
+        <v>7.3423150526877192</v>
       </c>
       <c r="F23">
         <f t="shared" si="1"/>
-        <v>0.25413719062986501</v>
+        <v>0.10489021503839599</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>55</v>
@@ -2027,11 +2232,11 @@
       </c>
       <c r="E24">
         <f t="shared" si="0"/>
-        <v>2.9279608447949559</v>
+        <v>3.1467064511518799</v>
       </c>
       <c r="F24">
         <f t="shared" si="1"/>
-        <v>0.14013780493475222</v>
+        <v>0.10489021503839599</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -2049,11 +2254,11 @@
       </c>
       <c r="E25">
         <f t="shared" si="0"/>
-        <v>0.78078955861198829</v>
+        <v>0.83912172030716792</v>
       </c>
       <c r="F25">
         <f t="shared" si="1"/>
-        <v>0.10121590264610075</v>
+        <v>0.10489021503839599</v>
       </c>
       <c r="H25" s="8" t="s">
         <v>56</v>
@@ -2076,15 +2281,15 @@
         <v>3.4000000000000002E-4</v>
       </c>
       <c r="D26">
-        <v>1E-4</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="E26">
         <f t="shared" si="0"/>
-        <v>0.33183556241009499</v>
+        <v>0.35662673113054638</v>
       </c>
       <c r="F26">
         <f>SQRT((D26*$H$18)^2+(C26*$I$18)^2)</f>
-        <v>9.8261907023536321E-2</v>
+        <v>1.04890215038396E-2</v>
       </c>
       <c r="H26">
         <v>0</v>
@@ -2113,11 +2318,11 @@
       </c>
       <c r="E27">
         <f t="shared" si="0"/>
-        <v>1.4639804223974779</v>
+        <v>1.5733532255759399</v>
       </c>
       <c r="F27">
         <f t="shared" si="1"/>
-        <v>0.10978970815545352</v>
+        <v>0.10489021503839599</v>
       </c>
       <c r="H27">
         <v>45</v>
@@ -2128,7 +2333,7 @@
       </c>
       <c r="J27">
         <f>D26</f>
-        <v>1E-4</v>
+        <v>1.0000000000000001E-5</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -2146,11 +2351,11 @@
       </c>
       <c r="E28">
         <f t="shared" si="0"/>
-        <v>4.6847373516719291</v>
+        <v>5.0347303218430071</v>
       </c>
       <c r="F28">
         <f t="shared" si="1"/>
-        <v>0.18818883875107567</v>
+        <v>0.10489021503839599</v>
       </c>
       <c r="H28">
         <v>90</v>
@@ -2179,11 +2384,11 @@
       </c>
       <c r="E29">
         <f t="shared" si="0"/>
-        <v>8.5886851447318708</v>
+        <v>9.2303389233788469</v>
       </c>
       <c r="F29">
         <f t="shared" si="1"/>
-        <v>0.31071386345629887</v>
+        <v>0.10489021503839599</v>
       </c>
       <c r="H29">
         <v>135</v>
@@ -2194,7 +2399,7 @@
       </c>
       <c r="J29">
         <f>D62</f>
-        <v>1E-4</v>
+        <v>1.0000000000000001E-5</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -2212,11 +2417,11 @@
       </c>
       <c r="E30">
         <f t="shared" si="0"/>
-        <v>15.615791172239764</v>
+        <v>16.782434406143359</v>
       </c>
       <c r="F30">
         <f t="shared" si="1"/>
-        <v>1.113648063723536</v>
+        <v>1.04890215038396</v>
       </c>
       <c r="H30">
         <v>180</v>
@@ -2245,11 +2450,11 @@
       </c>
       <c r="E31">
         <f t="shared" si="0"/>
-        <v>22.447699810094662</v>
+        <v>24.124749458831076</v>
       </c>
       <c r="F31">
         <f t="shared" si="1"/>
-        <v>1.2437749061163437</v>
+        <v>1.04890215038396</v>
       </c>
       <c r="H31">
         <v>225</v>
@@ -2260,7 +2465,7 @@
       </c>
       <c r="J31">
         <f>D98</f>
-        <v>1E-4</v>
+        <v>1.0000000000000001E-5</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -2278,11 +2483,11 @@
       </c>
       <c r="E32">
         <f t="shared" si="0"/>
-        <v>31.231582344479527</v>
+        <v>33.564868812286718</v>
       </c>
       <c r="F32">
         <f t="shared" si="1"/>
-        <v>1.4502401421109288</v>
+        <v>1.04890215038396</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -2300,11 +2505,11 @@
       </c>
       <c r="E33">
         <f t="shared" si="0"/>
-        <v>40.0154648788644</v>
+        <v>43.004988165742361</v>
       </c>
       <c r="F33">
         <f t="shared" si="1"/>
-        <v>1.6856609110425615</v>
+        <v>1.04890215038396</v>
       </c>
       <c r="I33" s="8" t="s">
         <v>34</v>
@@ -2328,11 +2533,11 @@
       </c>
       <c r="E34">
         <f t="shared" si="0"/>
-        <v>49.775334361514247</v>
+        <v>53.494009669581949</v>
       </c>
       <c r="F34">
         <f t="shared" si="1"/>
-        <v>1.9685619560153447</v>
+        <v>1.04890215038396</v>
       </c>
       <c r="H34" t="s">
         <v>59</v>
@@ -2361,22 +2566,22 @@
       </c>
       <c r="E35">
         <f t="shared" si="0"/>
-        <v>59.535203844164101</v>
+        <v>63.983031173421551</v>
       </c>
       <c r="F35">
         <f t="shared" si="1"/>
-        <v>2.2657791548982948</v>
+        <v>1.04890215038396</v>
       </c>
       <c r="H35" t="s">
         <v>60</v>
       </c>
       <c r="I35">
         <f>(I27/J27^2+I29/J29^2+I31/J31^2)/(1/J27^2+1/J29^2+1/J31^2)</f>
-        <v>5.1333333333333331E-4</v>
+        <v>5.1333333333333341E-4</v>
       </c>
       <c r="J35">
         <f>SQRT(3/(1/J27^2+1/J29^2+1/J31^2))</f>
-        <v>1E-4</v>
+        <v>1.0000000000000001E-5</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -2394,11 +2599,11 @@
       </c>
       <c r="E36">
         <f t="shared" si="0"/>
-        <v>70.271060275078938</v>
+        <v>75.520954827645113</v>
       </c>
       <c r="F36">
         <f t="shared" si="1"/>
-        <v>2.6034007812624882</v>
+        <v>1.04890215038396</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -2416,22 +2621,22 @@
       </c>
       <c r="E37">
         <f t="shared" si="0"/>
-        <v>78.078955861198821</v>
+        <v>83.912172030716789</v>
       </c>
       <c r="F37">
         <f t="shared" si="1"/>
-        <v>2.8537848008343496</v>
+        <v>1.04890215038396</v>
       </c>
       <c r="H37" t="s">
         <v>61</v>
       </c>
       <c r="I37">
         <f>I34/I35</f>
-        <v>229.22077922077924</v>
+        <v>229.22077922077918</v>
       </c>
       <c r="J37">
         <f>SQRT((J34/I35)^2+(I34*J35/I35^2)^2)</f>
-        <v>44.695871268082655</v>
+        <v>4.8717724097617747</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -2449,11 +2654,11 @@
       </c>
       <c r="E38">
         <f t="shared" si="0"/>
-        <v>87.838825343848669</v>
+        <v>94.401193534556384</v>
       </c>
       <c r="F38">
         <f t="shared" si="1"/>
-        <v>3.1708578885325034</v>
+        <v>1.04890215038396</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -2471,11 +2676,11 @@
       </c>
       <c r="E39">
         <f t="shared" si="0"/>
-        <v>94.670733981703577</v>
+        <v>101.74350858724411</v>
       </c>
       <c r="F39">
         <f t="shared" si="1"/>
-        <v>3.394883478900486</v>
+        <v>1.04890215038396</v>
       </c>
     </row>
     <row r="40" spans="1:10">
@@ -2493,11 +2698,11 @@
       </c>
       <c r="E40">
         <f t="shared" si="0"/>
-        <v>102.47862956782345</v>
+        <v>110.13472579031578</v>
       </c>
       <c r="F40">
         <f t="shared" si="1"/>
-        <v>3.6525466417007708</v>
+        <v>1.04890215038396</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -2515,11 +2720,11 @@
       </c>
       <c r="E41">
         <f t="shared" si="0"/>
-        <v>107.35856430914838</v>
+        <v>115.37923654223559</v>
       </c>
       <c r="F41">
         <f t="shared" si="1"/>
-        <v>3.8143217586092257</v>
+        <v>1.04890215038396</v>
       </c>
     </row>
     <row r="42" spans="1:10">
@@ -2537,11 +2742,11 @@
       </c>
       <c r="E42">
         <f t="shared" si="0"/>
-        <v>112.23849905047331</v>
+        <v>120.62374729415539</v>
       </c>
       <c r="F42">
         <f t="shared" si="1"/>
-        <v>3.9765799213283279</v>
+        <v>1.04890215038396</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -2559,11 +2764,11 @@
       </c>
       <c r="E43">
         <f t="shared" si="0"/>
-        <v>114.19047294700329</v>
+        <v>122.72155159492331</v>
       </c>
       <c r="F43">
         <f t="shared" si="1"/>
-        <v>4.04160541310846</v>
+        <v>1.04890215038396</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -2581,11 +2786,11 @@
       </c>
       <c r="E44">
         <f t="shared" si="0"/>
-        <v>114.19047294700329</v>
+        <v>122.72155159492331</v>
       </c>
       <c r="F44">
         <f t="shared" si="1"/>
-        <v>4.04160541310846</v>
+        <v>1.04890215038396</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -2603,11 +2808,11 @@
       </c>
       <c r="E45">
         <f t="shared" si="0"/>
-        <v>113.2144859987383</v>
+        <v>121.67264944453936</v>
       </c>
       <c r="F45">
         <f t="shared" si="1"/>
-        <v>4.0090843612110953</v>
+        <v>1.04890215038396</v>
       </c>
     </row>
     <row r="46" spans="1:10">
@@ -2625,11 +2830,11 @@
       </c>
       <c r="E46">
         <f t="shared" si="0"/>
-        <v>110.28652515394333</v>
+        <v>118.52594299338747</v>
       </c>
       <c r="F46">
         <f t="shared" si="1"/>
-        <v>3.9116225338871184</v>
+        <v>1.04890215038396</v>
       </c>
     </row>
     <row r="47" spans="1:10">
@@ -2647,11 +2852,11 @@
       </c>
       <c r="E47">
         <f t="shared" si="0"/>
-        <v>106.38257736088339</v>
+        <v>114.33033439185164</v>
       </c>
       <c r="F47">
         <f t="shared" si="1"/>
-        <v>3.7819261052790027</v>
+        <v>1.04890215038396</v>
       </c>
     </row>
     <row r="48" spans="1:10">
@@ -2669,11 +2874,11 @@
       </c>
       <c r="E48">
         <f t="shared" si="0"/>
-        <v>99.550668723028494</v>
+        <v>106.9880193391639</v>
       </c>
       <c r="F48">
         <f t="shared" si="1"/>
-        <v>3.5557408692328862</v>
+        <v>1.04890215038396</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -2691,11 +2896,11 @@
       </c>
       <c r="E49">
         <f t="shared" si="0"/>
-        <v>92.718760085173599</v>
+        <v>99.645704286476189</v>
       </c>
       <c r="F49">
         <f t="shared" si="1"/>
-        <v>3.3307268884335284</v>
+        <v>1.04890215038396</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -2713,11 +2918,11 @@
       </c>
       <c r="E50">
         <f t="shared" si="0"/>
-        <v>84.910864499053716</v>
+        <v>91.254487083404499</v>
       </c>
       <c r="F50">
         <f t="shared" si="1"/>
-        <v>3.0753319983382639</v>
+        <v>1.04890215038396</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -2735,11 +2940,11 @@
       </c>
       <c r="E51">
         <f t="shared" si="0"/>
-        <v>76.126981964668843</v>
+        <v>81.81436772994887</v>
       </c>
       <c r="F51">
         <f t="shared" si="1"/>
-        <v>2.7908789909072733</v>
+        <v>1.04890215038396</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -2757,11 +2962,11 @@
       </c>
       <c r="E52">
         <f t="shared" si="0"/>
-        <v>65.391125533754021</v>
+        <v>70.276444075725323</v>
       </c>
       <c r="F52">
         <f t="shared" si="1"/>
-        <v>2.4488241338908718</v>
+        <v>1.04890215038396</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -2779,11 +2984,11 @@
       </c>
       <c r="E53">
         <f t="shared" si="0"/>
-        <v>56.607242999369149</v>
+        <v>60.83632472226968</v>
       </c>
       <c r="F53">
         <f t="shared" si="1"/>
-        <v>2.1754544918739493</v>
+        <v>1.04890215038396</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -2801,11 +3006,11 @@
       </c>
       <c r="E54">
         <f t="shared" si="0"/>
-        <v>44.895399620189323</v>
+        <v>48.249498917662152</v>
       </c>
       <c r="F54">
         <f t="shared" si="1"/>
-        <v>1.8248979420197944</v>
+        <v>1.04890215038396</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -2823,11 +3028,11 @@
       </c>
       <c r="E55">
         <f t="shared" si="0"/>
-        <v>38.063490982334422</v>
+        <v>40.907183864974435</v>
       </c>
       <c r="F55">
         <f t="shared" si="1"/>
-        <v>1.6314607803620653</v>
+        <v>1.04890215038396</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -2845,11 +3050,11 @@
       </c>
       <c r="E56">
         <f t="shared" si="0"/>
-        <v>27.327634551419589</v>
+        <v>29.369260210750877</v>
       </c>
       <c r="F56">
         <f t="shared" si="1"/>
-        <v>1.3540730504865934</v>
+        <v>1.04890215038396</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -2867,11 +3072,11 @@
       </c>
       <c r="E57">
         <f t="shared" si="0"/>
-        <v>20.495725913564691</v>
+        <v>22.02694515806316</v>
       </c>
       <c r="F57">
         <f t="shared" si="1"/>
-        <v>1.2033671015314646</v>
+        <v>1.04890215038396</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -2889,11 +3094,11 @@
       </c>
       <c r="E58">
         <f t="shared" si="0"/>
-        <v>12.687830327444807</v>
+        <v>13.635727954991479</v>
       </c>
       <c r="F58">
         <f t="shared" si="1"/>
-        <v>1.0688554867150808</v>
+        <v>1.04890215038396</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -2911,11 +3116,11 @@
       </c>
       <c r="E59">
         <f t="shared" si="0"/>
-        <v>7.8078955861198818</v>
+        <v>8.3912172030716796</v>
       </c>
       <c r="F59">
         <f t="shared" si="1"/>
-        <v>0.28537848008343497</v>
+        <v>0.10489021503839599</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -2933,11 +3138,11 @@
       </c>
       <c r="E60">
         <f t="shared" si="0"/>
-        <v>3.9039477930599409</v>
+        <v>4.1956086015358398</v>
       </c>
       <c r="F60">
         <f t="shared" si="1"/>
-        <v>0.16584434915775656</v>
+        <v>0.10489021503839599</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -2955,11 +3160,11 @@
       </c>
       <c r="E61">
         <f t="shared" si="0"/>
-        <v>1.9519738965299704</v>
+        <v>2.0978043007679199</v>
       </c>
       <c r="F61">
         <f t="shared" si="1"/>
-        <v>0.11840699287105876</v>
+        <v>0.10489021503839599</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -2973,15 +3178,15 @@
         <v>8.0000000000000004E-4</v>
       </c>
       <c r="D62">
-        <v>1E-4</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="E62">
         <f t="shared" si="0"/>
-        <v>0.78078955861198829</v>
+        <v>0.83912172030716792</v>
       </c>
       <c r="F62">
         <f t="shared" si="1"/>
-        <v>0.10121590264610075</v>
+        <v>1.04890215038396E-2</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -2999,11 +3204,11 @@
       </c>
       <c r="E63">
         <f t="shared" si="0"/>
-        <v>1.854375201703472</v>
+        <v>1.9929140857295238</v>
       </c>
       <c r="F63">
         <f t="shared" si="1"/>
-        <v>0.11654175931697698</v>
+        <v>0.10489021503839599</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -3021,11 +3226,11 @@
       </c>
       <c r="E64">
         <f t="shared" si="0"/>
-        <v>4.8799347413249263</v>
+        <v>5.2445107519197993</v>
       </c>
       <c r="F64">
         <f t="shared" si="1"/>
-        <v>0.19395217783684343</v>
+        <v>0.10489021503839599</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -3043,11 +3248,11 @@
       </c>
       <c r="E65">
         <f t="shared" si="0"/>
-        <v>8.7838825343848672</v>
+        <v>9.4401193534556391</v>
       </c>
       <c r="F65">
         <f t="shared" si="1"/>
-        <v>0.31708578885325039</v>
+        <v>0.10489021503839599</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -3065,11 +3270,11 @@
       </c>
       <c r="E66">
         <f t="shared" si="0"/>
-        <v>15.615791172239764</v>
+        <v>16.782434406143359</v>
       </c>
       <c r="F66">
         <f t="shared" si="1"/>
-        <v>1.113648063723536</v>
+        <v>1.04890215038396</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -3087,11 +3292,11 @@
       </c>
       <c r="E67">
         <f t="shared" si="0"/>
-        <v>21.471712861829673</v>
+        <v>23.075847308447116</v>
       </c>
       <c r="F67">
         <f t="shared" si="1"/>
-        <v>1.2232785951631158</v>
+        <v>1.04890215038396</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -3109,11 +3314,11 @@
       </c>
       <c r="E68">
         <f t="shared" si="0"/>
-        <v>30.255595396214542</v>
+        <v>32.515966661902759</v>
       </c>
       <c r="F68">
         <f t="shared" si="1"/>
-        <v>1.4256243459653961</v>
+        <v>1.04890215038396</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -3131,11 +3336,11 @@
       </c>
       <c r="E69">
         <f t="shared" si="0"/>
-        <v>39.039477930599411</v>
+        <v>41.956086015358395</v>
       </c>
       <c r="F69">
         <f t="shared" si="1"/>
-        <v>1.6584434915775654</v>
+        <v>1.04890215038396</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -3153,11 +3358,11 @@
       </c>
       <c r="E70">
         <f t="shared" si="0"/>
-        <v>48.799347413249265</v>
+        <v>52.445107519197997</v>
       </c>
       <c r="F70">
         <f t="shared" si="1"/>
-        <v>1.9395217783684342</v>
+        <v>1.04890215038396</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -3175,11 +3380,11 @@
       </c>
       <c r="E71">
         <f t="shared" si="0"/>
-        <v>58.559216895899112</v>
+        <v>62.934129023037592</v>
       </c>
       <c r="F71">
         <f t="shared" si="1"/>
-        <v>2.2355737919427909</v>
+        <v>1.04890215038396</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -3197,11 +3402,11 @@
       </c>
       <c r="E72">
         <f t="shared" si="0"/>
-        <v>69.295073326813949</v>
+        <v>74.472052677261146</v>
       </c>
       <c r="F72">
         <f t="shared" si="1"/>
-        <v>2.572354897621798</v>
+        <v>1.04890215038396</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -3219,11 +3424,11 @@
       </c>
       <c r="E73">
         <f t="shared" ref="E73:E98" si="2">C73*$H$18</f>
-        <v>78.078955861198821</v>
+        <v>83.912172030716789</v>
       </c>
       <c r="F73">
         <f t="shared" ref="F73:F98" si="3">SQRT((D73*$H$18)^2+(C73*$I$18)^2)</f>
-        <v>2.8537848008343496</v>
+        <v>1.04890215038396</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -3241,11 +3446,11 @@
       </c>
       <c r="E74">
         <f t="shared" si="2"/>
-        <v>87.838825343848669</v>
+        <v>94.401193534556384</v>
       </c>
       <c r="F74">
         <f t="shared" si="3"/>
-        <v>3.1708578885325034</v>
+        <v>1.04890215038396</v>
       </c>
     </row>
     <row r="75" spans="1:6">
@@ -3263,11 +3468,11 @@
       </c>
       <c r="E75">
         <f t="shared" si="2"/>
-        <v>94.670733981703577</v>
+        <v>101.74350858724411</v>
       </c>
       <c r="F75">
         <f t="shared" si="3"/>
-        <v>3.394883478900486</v>
+        <v>1.04890215038396</v>
       </c>
     </row>
     <row r="76" spans="1:6">
@@ -3285,11 +3490,11 @@
       </c>
       <c r="E76">
         <f t="shared" si="2"/>
-        <v>103.45461651608844</v>
+        <v>111.18362794069975</v>
       </c>
       <c r="F76">
         <f t="shared" si="3"/>
-        <v>3.684859964876642</v>
+        <v>1.04890215038396</v>
       </c>
     </row>
     <row r="77" spans="1:6">
@@ -3307,11 +3512,11 @@
       </c>
       <c r="E77">
         <f t="shared" si="2"/>
-        <v>108.33455125741337</v>
+        <v>116.42813869261956</v>
       </c>
       <c r="F77">
         <f t="shared" si="3"/>
-        <v>3.8467367008898874</v>
+        <v>1.04890215038396</v>
       </c>
     </row>
     <row r="78" spans="1:6">
@@ -3329,11 +3534,11 @@
       </c>
       <c r="E78">
         <f t="shared" si="2"/>
-        <v>112.23849905047331</v>
+        <v>120.62374729415539</v>
       </c>
       <c r="F78">
         <f t="shared" si="3"/>
-        <v>3.9765799213283279</v>
+        <v>1.04890215038396</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -3351,11 +3556,11 @@
       </c>
       <c r="E79">
         <f t="shared" si="2"/>
-        <v>114.19047294700329</v>
+        <v>122.72155159492331</v>
       </c>
       <c r="F79">
         <f t="shared" si="3"/>
-        <v>4.04160541310846</v>
+        <v>1.04890215038396</v>
       </c>
     </row>
     <row r="80" spans="1:6">
@@ -3373,11 +3578,11 @@
       </c>
       <c r="E80">
         <f t="shared" si="2"/>
-        <v>115.16645989526825</v>
+        <v>123.77045374530726</v>
       </c>
       <c r="F80">
         <f t="shared" si="3"/>
-        <v>4.0741426792139102</v>
+        <v>1.04890215038396</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -3395,11 +3600,11 @@
       </c>
       <c r="E81">
         <f t="shared" si="2"/>
-        <v>114.19047294700329</v>
+        <v>122.72155159492331</v>
       </c>
       <c r="F81">
         <f t="shared" si="3"/>
-        <v>4.04160541310846</v>
+        <v>1.04890215038396</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -3417,11 +3622,11 @@
       </c>
       <c r="E82">
         <f t="shared" si="2"/>
-        <v>110.28652515394333</v>
+        <v>118.52594299338747</v>
       </c>
       <c r="F82">
         <f t="shared" si="3"/>
-        <v>3.9116225338871184</v>
+        <v>1.04890215038396</v>
       </c>
     </row>
     <row r="83" spans="1:6">
@@ -3439,11 +3644,11 @@
       </c>
       <c r="E83">
         <f t="shared" si="2"/>
-        <v>107.35856430914838</v>
+        <v>115.37923654223559</v>
       </c>
       <c r="F83">
         <f t="shared" si="3"/>
-        <v>3.8143217586092257</v>
+        <v>1.04890215038396</v>
       </c>
     </row>
     <row r="84" spans="1:6">
@@ -3461,11 +3666,11 @@
       </c>
       <c r="E84">
         <f t="shared" si="2"/>
-        <v>99.550668723028494</v>
+        <v>106.9880193391639</v>
       </c>
       <c r="F84">
         <f t="shared" si="3"/>
-        <v>3.5557408692328862</v>
+        <v>1.04890215038396</v>
       </c>
     </row>
     <row r="85" spans="1:6">
@@ -3483,11 +3688,11 @@
       </c>
       <c r="E85">
         <f t="shared" si="2"/>
-        <v>93.694747033438588</v>
+        <v>100.69460643686016</v>
       </c>
       <c r="F85">
         <f t="shared" si="3"/>
-        <v>3.3627911089808338</v>
+        <v>1.04890215038396</v>
       </c>
     </row>
     <row r="86" spans="1:6">
@@ -3505,11 +3710,11 @@
       </c>
       <c r="E86">
         <f t="shared" si="2"/>
-        <v>83.934877550788727</v>
+        <v>90.205584933020546</v>
       </c>
       <c r="F86">
         <f t="shared" si="3"/>
-        <v>3.0435621664386874</v>
+        <v>1.04890215038396</v>
       </c>
     </row>
     <row r="87" spans="1:6">
@@ -3527,11 +3732,11 @@
       </c>
       <c r="E87">
         <f t="shared" si="2"/>
-        <v>76.126981964668843</v>
+        <v>81.81436772994887</v>
       </c>
       <c r="F87">
         <f t="shared" si="3"/>
-        <v>2.7908789909072733</v>
+        <v>1.04890215038396</v>
       </c>
     </row>
     <row r="88" spans="1:6">
@@ -3549,11 +3754,11 @@
       </c>
       <c r="E88">
         <f t="shared" si="2"/>
-        <v>65.391125533754021</v>
+        <v>70.276444075725323</v>
       </c>
       <c r="F88">
         <f t="shared" si="3"/>
-        <v>2.4488241338908718</v>
+        <v>1.04890215038396</v>
       </c>
     </row>
     <row r="89" spans="1:6">
@@ -3571,11 +3776,11 @@
       </c>
       <c r="E89">
         <f t="shared" si="2"/>
-        <v>56.607242999369149</v>
+        <v>60.83632472226968</v>
       </c>
       <c r="F89">
         <f t="shared" si="3"/>
-        <v>2.1754544918739493</v>
+        <v>1.04890215038396</v>
       </c>
     </row>
     <row r="90" spans="1:6">
@@ -3593,11 +3798,11 @@
       </c>
       <c r="E90">
         <f t="shared" si="2"/>
-        <v>44.895399620189323</v>
+        <v>48.249498917662152</v>
       </c>
       <c r="F90">
         <f t="shared" si="3"/>
-        <v>1.8248979420197944</v>
+        <v>1.04890215038396</v>
       </c>
     </row>
     <row r="91" spans="1:6">
@@ -3615,11 +3820,11 @@
       </c>
       <c r="E91">
         <f t="shared" si="2"/>
-        <v>38.063490982334422</v>
+        <v>40.907183864974435</v>
       </c>
       <c r="F91">
         <f t="shared" si="3"/>
-        <v>1.6314607803620653</v>
+        <v>1.04890215038396</v>
       </c>
     </row>
     <row r="92" spans="1:6">
@@ -3637,11 +3842,11 @@
       </c>
       <c r="E92">
         <f t="shared" si="2"/>
-        <v>27.327634551419589</v>
+        <v>29.369260210750877</v>
       </c>
       <c r="F92">
         <f t="shared" si="3"/>
-        <v>1.3540730504865934</v>
+        <v>1.04890215038396</v>
       </c>
     </row>
     <row r="93" spans="1:6">
@@ -3659,11 +3864,11 @@
       </c>
       <c r="E93">
         <f t="shared" si="2"/>
-        <v>19.519738965299705</v>
+        <v>20.978043007679197</v>
       </c>
       <c r="F93">
         <f t="shared" si="3"/>
-        <v>1.1840699287105876</v>
+        <v>1.04890215038396</v>
       </c>
     </row>
     <row r="94" spans="1:6">
@@ -3681,11 +3886,11 @@
       </c>
       <c r="E94">
         <f t="shared" si="2"/>
-        <v>12.687830327444807</v>
+        <v>13.635727954991479</v>
       </c>
       <c r="F94">
         <f t="shared" si="3"/>
-        <v>1.0688554867150808</v>
+        <v>1.04890215038396</v>
       </c>
     </row>
     <row r="95" spans="1:6">
@@ -3703,11 +3908,11 @@
       </c>
       <c r="E95">
         <f t="shared" si="2"/>
-        <v>7.8078955861198818</v>
+        <v>8.3912172030716796</v>
       </c>
       <c r="F95">
         <f t="shared" si="3"/>
-        <v>0.28537848008343497</v>
+        <v>0.10489021503839599</v>
       </c>
     </row>
     <row r="96" spans="1:6">
@@ -3725,11 +3930,11 @@
       </c>
       <c r="E96">
         <f t="shared" si="2"/>
-        <v>3.9039477930599409</v>
+        <v>4.1956086015358398</v>
       </c>
       <c r="F96">
         <f t="shared" si="3"/>
-        <v>0.16584434915775656</v>
+        <v>0.10489021503839599</v>
       </c>
     </row>
     <row r="97" spans="1:6">
@@ -3747,11 +3952,11 @@
       </c>
       <c r="E97">
         <f t="shared" si="2"/>
-        <v>0.97598694826498522</v>
+        <v>1.04890215038396</v>
       </c>
       <c r="F97">
         <f t="shared" si="3"/>
-        <v>0.10319487833254484</v>
+        <v>0.10489021503839599</v>
       </c>
     </row>
     <row r="98" spans="1:6">
@@ -3765,15 +3970,15 @@
         <v>4.0000000000000002E-4</v>
       </c>
       <c r="D98">
-        <v>1E-4</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="E98">
         <f t="shared" si="2"/>
-        <v>0.39039477930599414</v>
+        <v>0.41956086015358396</v>
       </c>
       <c r="F98">
         <f t="shared" si="3"/>
-        <v>9.8515448844296652E-2</v>
+        <v>1.04890215038396E-2</v>
       </c>
     </row>
   </sheetData>
@@ -3815,7 +4020,7 @@
   <dimension ref="A1:K70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -5523,7 +5728,7 @@
   <dimension ref="A1:N81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -10096,7 +10301,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
@@ -10330,1065 +10535,2022 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="F1:I75"/>
+  <dimension ref="A1:F91"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:I1048576"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="4" width="11.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="13"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="6:9">
-      <c r="F1">
-        <v>112.553</v>
-      </c>
-      <c r="G1">
-        <v>0.37819999999999998</v>
-      </c>
-      <c r="H1">
-        <v>23.7</v>
-      </c>
-      <c r="I1">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="2" spans="6:9">
-      <c r="F2">
-        <v>111.693987190893</v>
-      </c>
-      <c r="G2">
-        <v>0.78148028788541435</v>
-      </c>
-      <c r="H2">
-        <v>23</v>
-      </c>
-      <c r="I2">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="3" spans="6:9">
-      <c r="F3">
-        <v>109.1431729603935</v>
-      </c>
-      <c r="G3">
-        <v>1.3989182962915241</v>
-      </c>
-      <c r="H3">
-        <v>21.4</v>
-      </c>
-      <c r="I3">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="4" spans="6:9">
-      <c r="F4">
-        <v>104.9784293189374</v>
-      </c>
-      <c r="G4">
-        <v>2.0045938492086832</v>
-      </c>
-      <c r="H4">
-        <v>19.600000000000001</v>
-      </c>
-      <c r="I4">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="5" spans="6:9">
-      <c r="F5">
-        <v>99.32689879083452</v>
-      </c>
-      <c r="G5">
-        <v>2.5582646947136163</v>
-      </c>
-      <c r="H5">
+    <row r="1" spans="1:6">
+      <c r="A1" s="13">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="13">
+        <v>1</v>
+      </c>
+      <c r="D1" s="13">
+        <v>1</v>
+      </c>
+      <c r="E1" s="13">
+        <f>C1*1000</f>
+        <v>1000</v>
+      </c>
+      <c r="F1" s="13">
+        <f>D1*1000</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="13">
+        <v>2.5</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="13">
+        <v>1</v>
+      </c>
+      <c r="D2" s="13">
+        <v>1</v>
+      </c>
+      <c r="E2" s="13">
+        <f t="shared" ref="E2:F65" si="0">C2*1000</f>
+        <v>1000</v>
+      </c>
+      <c r="F2" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="13">
+        <v>5</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" s="13">
+        <v>1</v>
+      </c>
+      <c r="D3" s="13">
+        <v>1</v>
+      </c>
+      <c r="E3" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="F3" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="13">
+        <v>7.5</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="13">
+        <v>1</v>
+      </c>
+      <c r="D4" s="13">
+        <v>1</v>
+      </c>
+      <c r="E4" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="F4" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="13">
+        <v>10</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" s="13">
+        <v>1</v>
+      </c>
+      <c r="D5" s="13">
+        <v>1</v>
+      </c>
+      <c r="E5" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="F5" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="13">
+        <v>12.5</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="C6" s="13">
+        <v>1</v>
+      </c>
+      <c r="D6" s="13">
+        <v>1</v>
+      </c>
+      <c r="E6" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="F6" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="13">
+        <v>15</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" s="13">
+        <v>1</v>
+      </c>
+      <c r="D7" s="13">
+        <v>1</v>
+      </c>
+      <c r="E7" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="F7" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="13">
         <v>17.5</v>
       </c>
-      <c r="I5">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="6" spans="6:9">
-      <c r="F6">
-        <v>92.361112969723337</v>
-      </c>
-      <c r="G6">
-        <v>3.037954364508034</v>
-      </c>
-      <c r="H6">
-        <v>15.3</v>
-      </c>
-      <c r="I6">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="7" spans="6:9">
-      <c r="F7">
-        <v>84.293725423108256</v>
-      </c>
-      <c r="G7">
-        <v>3.4271936217363717</v>
-      </c>
-      <c r="H7">
-        <v>12.6</v>
-      </c>
-      <c r="I7">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="8" spans="6:9">
-      <c r="F8">
-        <v>75.371019741424803</v>
-      </c>
-      <c r="G8">
-        <v>3.7132629587734853</v>
-      </c>
-      <c r="H8">
-        <v>9.9</v>
-      </c>
-      <c r="I8">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="9" spans="6:9">
-      <c r="F9">
-        <v>65.865390919829281</v>
-      </c>
-      <c r="G9">
-        <v>3.8869796423982366</v>
-      </c>
-      <c r="H9">
-        <v>7</v>
-      </c>
-      <c r="I9">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="10" spans="6:9">
-      <c r="F10">
-        <v>56.067029603310949</v>
-      </c>
-      <c r="G10">
-        <v>3.9427695282759787</v>
-      </c>
-      <c r="H10">
-        <v>5.2</v>
-      </c>
-      <c r="I10">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="11" spans="6:9">
-      <c r="F11">
-        <v>46.27506306094822</v>
-      </c>
-      <c r="G11">
-        <v>3.8787510651947663</v>
-      </c>
-      <c r="H11">
-        <v>3.5</v>
-      </c>
-      <c r="I11">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="12" spans="6:9">
-      <c r="F12">
-        <v>36.788423340264913</v>
-      </c>
-      <c r="G12">
-        <v>3.696752369519364</v>
-      </c>
-      <c r="H12">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="I12">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="13" spans="6:9">
-      <c r="F13">
-        <v>27.896721381367488</v>
-      </c>
-      <c r="G13">
-        <v>3.4022346269051393</v>
-      </c>
-      <c r="H13">
-        <v>1.3</v>
-      </c>
-      <c r="I13">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="14" spans="6:9">
-      <c r="F14">
-        <v>19.871405688603378</v>
-      </c>
-      <c r="G14">
-        <v>3.0041138395583999</v>
-      </c>
-      <c r="H14">
-        <v>0.8</v>
-      </c>
-      <c r="I14">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="15" spans="6:9">
-      <c r="F15">
-        <v>12.957475470424107</v>
-      </c>
-      <c r="G15">
-        <v>2.5144818402151099</v>
-      </c>
-      <c r="H15">
-        <v>0.4</v>
-      </c>
-      <c r="I15">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="16" spans="6:9">
-      <c r="F16">
-        <v>7.3660012311676759</v>
-      </c>
-      <c r="G16">
-        <v>1.948232931073471</v>
-      </c>
-      <c r="H16">
-        <v>0.2</v>
-      </c>
-      <c r="I16">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="17" spans="6:9">
-      <c r="F17">
-        <v>3.2676811483437938</v>
-      </c>
-      <c r="G17">
-        <v>1.322606436529951</v>
-      </c>
-      <c r="H17">
-        <v>0.11</v>
-      </c>
-      <c r="I17">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="18" spans="6:9">
-      <c r="F18">
-        <v>0.78762994824019816</v>
-      </c>
-      <c r="G18">
-        <v>0.65665852544455006</v>
-      </c>
-      <c r="H18">
-        <v>0.09</v>
-      </c>
-      <c r="I18">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="19" spans="6:9">
-      <c r="F19">
-        <v>1.5593665949043955E-3</v>
-      </c>
-      <c r="G19">
-        <v>2.9320931119283793E-2</v>
-      </c>
-      <c r="H19">
-        <v>0.09</v>
-      </c>
-      <c r="I19">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="20" spans="6:9">
-      <c r="F20">
-        <v>0.93346679835946744</v>
-      </c>
-      <c r="G20">
-        <v>0.71442889299342249</v>
-      </c>
-      <c r="H20">
-        <v>0.13</v>
-      </c>
-      <c r="I20">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="21" spans="6:9">
-      <c r="F21">
-        <v>3.5549026981361496</v>
-      </c>
-      <c r="G21">
-        <v>1.3777882938644588</v>
-      </c>
-      <c r="H21">
-        <v>0.24</v>
-      </c>
-      <c r="I21">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="22" spans="6:9">
-      <c r="F22">
-        <v>7.7858390963049153</v>
-      </c>
-      <c r="G22">
-        <v>1.9991864173081153</v>
-      </c>
-      <c r="H22">
-        <v>0.44</v>
-      </c>
-      <c r="I22">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="23" spans="6:9">
-      <c r="F23">
-        <v>13.497112716523288</v>
-      </c>
-      <c r="G23">
-        <v>2.5596931530233067</v>
-      </c>
-      <c r="H23">
-        <v>0.9</v>
-      </c>
-      <c r="I23">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="24" spans="6:9">
-      <c r="F24">
-        <v>20.514368110386236</v>
-      </c>
-      <c r="G24">
-        <v>3.0422404237141905</v>
-      </c>
-      <c r="H24">
-        <v>1.58</v>
-      </c>
-      <c r="I24">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="25" spans="6:9">
-      <c r="F25">
-        <v>28.623380432066348</v>
-      </c>
-      <c r="G25">
-        <v>3.4321453271878202</v>
-      </c>
-      <c r="H25">
-        <v>2.81</v>
-      </c>
-      <c r="I25">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="26" spans="6:9">
-      <c r="F26">
-        <v>37.576595357697379</v>
-      </c>
-      <c r="G26">
-        <v>3.7175613925695852</v>
-      </c>
-      <c r="H26">
-        <v>3.9</v>
-      </c>
-      <c r="I26">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="27" spans="6:9">
-      <c r="F27">
-        <v>47.100686496910164</v>
-      </c>
-      <c r="G27">
-        <v>3.8898448086638835</v>
-      </c>
-      <c r="H27">
-        <v>6.3</v>
-      </c>
-      <c r="I27">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="28" spans="6:9">
-      <c r="F28">
-        <v>56.904899581628847</v>
-      </c>
-      <c r="G28">
-        <v>3.9438256083629719</v>
-      </c>
-      <c r="H28">
-        <v>9</v>
-      </c>
-      <c r="I28">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="29" spans="6:9">
-      <c r="F29">
-        <v>66.689928698266499</v>
-      </c>
-      <c r="G29">
-        <v>3.8779778145166532</v>
-      </c>
-      <c r="H29">
-        <v>12.5</v>
-      </c>
-      <c r="I29">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="30" spans="6:9">
-      <c r="F30">
-        <v>76.157053587081407</v>
-      </c>
-      <c r="G30">
-        <v>3.6944881755525207</v>
-      </c>
-      <c r="H30">
-        <v>15.9</v>
-      </c>
-      <c r="I30">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="31" spans="6:9">
-      <c r="F31">
-        <v>85.017259062519813</v>
-      </c>
-      <c r="G31">
-        <v>3.399232501308628</v>
-      </c>
-      <c r="H31">
-        <v>19</v>
-      </c>
-      <c r="I31">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="32" spans="6:9">
-      <c r="F32">
-        <v>93.000058154186604</v>
-      </c>
-      <c r="G32">
-        <v>3.00168885330593</v>
-      </c>
-      <c r="H32">
-        <v>21</v>
-      </c>
-      <c r="I32">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="33" spans="6:9">
-      <c r="F33">
-        <v>99.861749612989527</v>
-      </c>
-      <c r="G33">
-        <v>2.5148747145630668</v>
-      </c>
-      <c r="H33">
-        <v>23.5</v>
-      </c>
-      <c r="I33">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="34" spans="6:9">
-      <c r="F34">
-        <v>105.39285769487017</v>
-      </c>
-      <c r="G34">
-        <v>1.9556143558971697</v>
-      </c>
-      <c r="H34">
-        <v>25.4</v>
-      </c>
-      <c r="I34">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="35" spans="6:9">
-      <c r="F35">
-        <v>109.42452709820567</v>
-      </c>
-      <c r="G35">
-        <v>1.346597798918223</v>
-      </c>
-      <c r="H35">
-        <v>26.7</v>
-      </c>
-      <c r="I35">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="36" spans="6:9">
-      <c r="F36">
-        <v>111.83367782834283</v>
-      </c>
-      <c r="G36">
-        <v>0.73183388137707039</v>
-      </c>
-      <c r="H36">
-        <v>27.3</v>
-      </c>
-      <c r="I36">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="37" spans="6:9">
-      <c r="F37">
-        <v>112.54676262003741</v>
-      </c>
-      <c r="G37">
-        <v>0.38270229986474558</v>
-      </c>
-      <c r="H37">
-        <v>26.6</v>
-      </c>
-      <c r="I37">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="38" spans="6:9">
-      <c r="F38">
-        <v>111.5420122100963</v>
-      </c>
-      <c r="G38">
-        <v>0.83269216227488452</v>
-      </c>
-      <c r="H38">
-        <v>25.5</v>
-      </c>
-      <c r="I38">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="39" spans="6:9">
-      <c r="F39">
-        <v>108.85009991587557</v>
-      </c>
-      <c r="G39">
-        <v>1.452624218754506</v>
-      </c>
-      <c r="H39">
-        <v>23.5</v>
-      </c>
-      <c r="I39">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="40" spans="6:9">
-      <c r="F40">
-        <v>104.55320523118627</v>
-      </c>
-      <c r="G40">
-        <v>2.0554481128725173</v>
-      </c>
-      <c r="H40">
-        <v>21.2</v>
-      </c>
-      <c r="I40">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="41" spans="6:9">
-      <c r="F41">
-        <v>98.782505026428339</v>
-      </c>
-      <c r="G41">
-        <v>2.6040386009568768</v>
-      </c>
-      <c r="H41">
-        <v>18.2</v>
-      </c>
-      <c r="I41">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="42" spans="6:9">
-      <c r="F42">
-        <v>91.714168942336499</v>
-      </c>
-      <c r="G42">
-        <v>3.0770546664525704</v>
-      </c>
-      <c r="H42">
-        <v>15.9</v>
-      </c>
-      <c r="I42">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="43" spans="6:9">
-      <c r="F43">
-        <v>83.56398123114063</v>
-      </c>
-      <c r="G43">
-        <v>3.4583567211228625</v>
-      </c>
-      <c r="H43">
-        <v>12.9</v>
-      </c>
-      <c r="I43">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="44" spans="6:9">
-      <c r="F44">
-        <v>74.580753231162916</v>
-      </c>
-      <c r="G44">
-        <v>3.7355089724648414</v>
-      </c>
-      <c r="H44">
-        <v>10.3</v>
-      </c>
-      <c r="I44">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="45" spans="6:9">
-      <c r="F45">
-        <v>65.038727580773113</v>
-      </c>
-      <c r="G45">
-        <v>3.8996148184147841</v>
-      </c>
-      <c r="H45">
-        <v>7.7</v>
-      </c>
-      <c r="I45">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="46" spans="6:9">
-      <c r="F46">
-        <v>55.229206058102911</v>
-      </c>
-      <c r="G46">
-        <v>3.9453964949989526</v>
-      </c>
-      <c r="H46">
-        <v>5.6</v>
-      </c>
-      <c r="I46">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="47" spans="6:9">
-      <c r="F47">
-        <v>45.451656634301344</v>
-      </c>
-      <c r="G47">
-        <v>3.8712760398958799</v>
-      </c>
-      <c r="H47">
-        <v>3.7</v>
-      </c>
-      <c r="I47">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="48" spans="6:9">
-      <c r="F48">
-        <v>36.00457122683742</v>
-      </c>
-      <c r="G48">
-        <v>3.6793856977295629</v>
-      </c>
-      <c r="H48">
-        <v>2.5</v>
-      </c>
-      <c r="I48">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="49" spans="6:9">
-      <c r="F49">
-        <v>27.176353250057659</v>
-      </c>
-      <c r="G49">
-        <v>3.3754833510840747</v>
-      </c>
-      <c r="H49">
-        <v>1.4</v>
-      </c>
-      <c r="I49">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="50" spans="6:9">
-      <c r="F50">
-        <v>19.236513150547925</v>
-      </c>
-      <c r="G50">
-        <v>2.9687659735731131</v>
-      </c>
-      <c r="H50">
-        <v>0.8</v>
-      </c>
-      <c r="I50">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="51" spans="6:9">
-      <c r="F51">
-        <v>12.427440712596237</v>
-      </c>
-      <c r="G51">
-        <v>2.4715825636206734</v>
-      </c>
-      <c r="H51">
-        <v>0.5</v>
-      </c>
-      <c r="I51">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="52" spans="6:9">
-      <c r="F52">
-        <v>6.9570053112466601</v>
-      </c>
-      <c r="G52">
-        <v>1.8990532830127793</v>
-      </c>
-      <c r="H52">
-        <v>0.3</v>
-      </c>
-      <c r="I52">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="53" spans="6:9">
-      <c r="F53">
-        <v>2.9922100146059414</v>
-      </c>
-      <c r="G53">
-        <v>1.2686053706798961</v>
-      </c>
-      <c r="H53">
-        <v>0.15</v>
-      </c>
-      <c r="I53">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="54" spans="6:9">
-      <c r="F54">
-        <v>0.65409326484085761</v>
-      </c>
-      <c r="G54">
-        <v>0.59943941400265666</v>
-      </c>
-      <c r="H54">
-        <v>0.11</v>
-      </c>
-      <c r="I54">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="55" spans="6:9">
-      <c r="F55">
-        <v>1.4033780856709617E-2</v>
-      </c>
-      <c r="G55">
-        <v>8.8058076076689015E-2</v>
-      </c>
-      <c r="H55">
-        <v>0.1</v>
-      </c>
-      <c r="I55">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="56" spans="6:9">
-      <c r="F56">
-        <v>1.0915714876784159</v>
-      </c>
-      <c r="G56">
-        <v>0.77293807685425264</v>
-      </c>
-      <c r="H56">
-        <v>0.13</v>
-      </c>
-      <c r="I56">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="57" spans="6:9">
-      <c r="F57">
-        <v>3.8538109958466054</v>
-      </c>
-      <c r="G57">
-        <v>1.434329581655547</v>
-      </c>
-      <c r="H57">
-        <v>0.26</v>
-      </c>
-      <c r="I57">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="58" spans="6:9">
-      <c r="F58">
-        <v>8.2164258415854778</v>
-      </c>
-      <c r="G58">
-        <v>2.0520778238707083</v>
-      </c>
-      <c r="H58">
-        <v>0.45</v>
-      </c>
-      <c r="I58">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="59" spans="6:9">
-      <c r="F59">
-        <v>14.046232830002412</v>
-      </c>
-      <c r="G59">
-        <v>2.607360849310544</v>
-      </c>
-      <c r="H59">
-        <v>0.91</v>
-      </c>
-      <c r="I59">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="60" spans="6:9">
-      <c r="F60">
-        <v>21.165257891008643</v>
-      </c>
-      <c r="G60">
-        <v>3.0832657805177064</v>
-      </c>
-      <c r="H60">
-        <v>1.64</v>
-      </c>
-      <c r="I60">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="61" spans="6:9">
-      <c r="F61">
-        <v>29.356169324311736</v>
-      </c>
-      <c r="G61">
-        <v>3.4653074189633855</v>
-      </c>
-      <c r="H61">
-        <v>2.79</v>
-      </c>
-      <c r="I61">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="62" spans="6:9">
-      <c r="F62">
-        <v>38.368912565769534</v>
-      </c>
-      <c r="G62">
-        <v>3.7418737340043298</v>
-      </c>
-      <c r="H62">
-        <v>4.1100000000000003</v>
-      </c>
-      <c r="I62">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="63" spans="6:9">
-      <c r="F63">
-        <v>47.928343927000604</v>
-      </c>
-      <c r="G63">
-        <v>3.9045852983381062</v>
-      </c>
-      <c r="H63">
-        <v>6.15</v>
-      </c>
-      <c r="I63">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="64" spans="6:9">
-      <c r="F64">
-        <v>57.742630263190236</v>
-      </c>
-      <c r="G64">
-        <v>3.9485589186984624</v>
-      </c>
-      <c r="H64">
-        <v>8.25</v>
-      </c>
-      <c r="I64">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="65" spans="6:9">
-      <c r="F65">
-        <v>67.512158141554764</v>
-      </c>
-      <c r="G65">
-        <v>3.8725698299061708</v>
-      </c>
-      <c r="H65">
-        <v>11</v>
-      </c>
-      <c r="I65">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="66" spans="6:9">
-      <c r="F66">
-        <v>76.938680528734082</v>
-      </c>
-      <c r="G66">
-        <v>3.6791126440206114</v>
-      </c>
-      <c r="H66">
-        <v>13.5</v>
-      </c>
-      <c r="I66">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="67" spans="6:9">
-      <c r="F67">
-        <v>85.734421764339771</v>
-      </c>
-      <c r="G67">
-        <v>3.374371149452331</v>
-      </c>
-      <c r="H67">
-        <v>16.5</v>
-      </c>
-      <c r="I67">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="68" spans="6:9">
-      <c r="F68">
-        <v>93.630862861335686</v>
-      </c>
-      <c r="G68">
-        <v>2.9681289280052252</v>
-      </c>
-      <c r="H68">
-        <v>18.600000000000001</v>
-      </c>
-      <c r="I68">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="69" spans="6:9">
-      <c r="F69">
-        <v>100.38693893300417</v>
-      </c>
-      <c r="G69">
-        <v>2.4737167711854156</v>
-      </c>
-      <c r="H69">
-        <v>21.3</v>
-      </c>
-      <c r="I69">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="70" spans="6:9">
-      <c r="F70">
-        <v>105.79639849302821</v>
-      </c>
-      <c r="G70">
-        <v>1.90834135664612</v>
-      </c>
-      <c r="H70">
-        <v>23.4</v>
-      </c>
-      <c r="I70">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="71" spans="6:9">
-      <c r="F71">
-        <v>109.69409996179957</v>
-      </c>
-      <c r="G71">
-        <v>1.2954952055306264</v>
-      </c>
-      <c r="H71">
+      <c r="B8" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" s="13">
+        <v>1</v>
+      </c>
+      <c r="D8" s="13">
+        <v>1</v>
+      </c>
+      <c r="E8" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="F8" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="13">
+        <v>20</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" s="13">
+        <v>1</v>
+      </c>
+      <c r="D9" s="13">
+        <v>1</v>
+      </c>
+      <c r="E9" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="F9" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="13">
+        <v>22.5</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10" s="13">
+        <v>1</v>
+      </c>
+      <c r="D10" s="13">
+        <v>1</v>
+      </c>
+      <c r="E10" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="F10" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="13">
         <v>25</v>
       </c>
-      <c r="I71">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="72" spans="6:9">
-      <c r="F72">
-        <v>111.96105315735076</v>
-      </c>
-      <c r="G72">
-        <v>0.68377301281808245</v>
-      </c>
-      <c r="H72">
-        <v>25.8</v>
-      </c>
-      <c r="I72">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="73" spans="6:9">
-      <c r="F73">
-        <v>112.52805186278395</v>
-      </c>
-      <c r="G73">
-        <v>0.39595858477958906</v>
-      </c>
-      <c r="H73">
-        <v>25.3</v>
-      </c>
-      <c r="I73">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="74" spans="6:9">
-      <c r="F74">
-        <v>111.37778657410672</v>
-      </c>
-      <c r="G74">
-        <v>0.88549313666107909</v>
-      </c>
-      <c r="H74">
-        <v>24.5</v>
-      </c>
-      <c r="I74">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="75" spans="6:9">
-      <c r="F75">
-        <v>108.54537292988387</v>
-      </c>
-      <c r="G75">
-        <v>1.5078783565021645</v>
-      </c>
-      <c r="H75">
-        <v>22.9</v>
-      </c>
-      <c r="I75">
-        <v>0.2</v>
+      <c r="B11" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="C11" s="13">
+        <v>1</v>
+      </c>
+      <c r="D11" s="13">
+        <v>1</v>
+      </c>
+      <c r="E11" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="F11" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="13">
+        <v>27.5</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="C12" s="13">
+        <v>1</v>
+      </c>
+      <c r="D12" s="13">
+        <v>1</v>
+      </c>
+      <c r="E12" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="F12" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="13">
+        <v>30</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C13" s="13">
+        <v>1</v>
+      </c>
+      <c r="D13" s="13">
+        <v>1</v>
+      </c>
+      <c r="E13" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="F13" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="13">
+        <v>32.5</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="C14" s="13">
+        <v>1</v>
+      </c>
+      <c r="D14" s="13">
+        <v>1</v>
+      </c>
+      <c r="E14" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="F14" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="13">
+        <v>35</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C15" s="13">
+        <v>1</v>
+      </c>
+      <c r="D15" s="13">
+        <v>1</v>
+      </c>
+      <c r="E15" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="F15" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="13">
+        <v>37.5</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="C16" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="D16" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="E16" s="13">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="F16" s="13">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="13">
+        <v>40</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="C17" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="D17" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="E17" s="13">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="F17" s="13">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="13">
+        <v>42.5</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="C18" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="D18" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="E18" s="13">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="F18" s="13">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="13">
+        <v>45</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="C19" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="D19" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="E19" s="13">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="F19" s="13">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="13">
+        <v>47.5</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="C20" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="D20" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="E20" s="13">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="F20" s="13">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="13">
+        <v>50</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="C21" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="D21" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="E21" s="13">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="F21" s="13">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="13">
+        <v>52.5</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="C22" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="D22" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="E22" s="13">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="F22" s="13">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="13">
+        <v>55</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="C23" s="13">
+        <v>1</v>
+      </c>
+      <c r="D23" s="13">
+        <v>1</v>
+      </c>
+      <c r="E23" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="F23" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="13">
+        <v>57.5</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="C24" s="13">
+        <v>1</v>
+      </c>
+      <c r="D24" s="13">
+        <v>1</v>
+      </c>
+      <c r="E24" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="F24" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="13">
+        <v>60</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="C25" s="13">
+        <v>1</v>
+      </c>
+      <c r="D25" s="13">
+        <v>1</v>
+      </c>
+      <c r="E25" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="F25" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="13">
+        <v>62.5</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="C26" s="13">
+        <v>1</v>
+      </c>
+      <c r="D26" s="13">
+        <v>1</v>
+      </c>
+      <c r="E26" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="F26" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="13">
+        <v>65</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="C27" s="13">
+        <v>1</v>
+      </c>
+      <c r="D27" s="13">
+        <v>1</v>
+      </c>
+      <c r="E27" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="F27" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="13">
+        <v>67.5</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="C28" s="13">
+        <v>1</v>
+      </c>
+      <c r="D28" s="13">
+        <v>1</v>
+      </c>
+      <c r="E28" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="F28" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="13">
+        <v>70</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="C29" s="13">
+        <v>1</v>
+      </c>
+      <c r="D29" s="13">
+        <v>1</v>
+      </c>
+      <c r="E29" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="F29" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="13">
+        <v>72.5</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="C30" s="13">
+        <v>1</v>
+      </c>
+      <c r="D30" s="13">
+        <v>1</v>
+      </c>
+      <c r="E30" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="F30" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="13">
+        <v>75</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C31" s="13">
+        <v>1</v>
+      </c>
+      <c r="D31" s="13">
+        <v>1</v>
+      </c>
+      <c r="E31" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="F31" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="13">
+        <v>77.5</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="C32" s="13">
+        <v>1</v>
+      </c>
+      <c r="D32" s="13">
+        <v>1</v>
+      </c>
+      <c r="E32" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="F32" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="13">
+        <v>80</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="C33" s="13">
+        <v>1</v>
+      </c>
+      <c r="D33" s="13">
+        <v>1</v>
+      </c>
+      <c r="E33" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="F33" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="13">
+        <v>82.5</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="C34" s="13">
+        <v>1</v>
+      </c>
+      <c r="D34" s="13">
+        <v>1</v>
+      </c>
+      <c r="E34" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="F34" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="13">
+        <v>85</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="C35" s="13">
+        <v>1</v>
+      </c>
+      <c r="D35" s="13">
+        <v>1</v>
+      </c>
+      <c r="E35" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="F35" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="13">
+        <v>87.5</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="C36" s="13">
+        <v>1</v>
+      </c>
+      <c r="D36" s="13">
+        <v>1</v>
+      </c>
+      <c r="E36" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="F36" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="13">
+        <v>90</v>
+      </c>
+      <c r="B37" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="C37" s="13">
+        <v>1</v>
+      </c>
+      <c r="D37" s="13">
+        <v>1</v>
+      </c>
+      <c r="E37" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="F37" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="13">
+        <v>92.5</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="C38" s="13">
+        <v>1</v>
+      </c>
+      <c r="D38" s="13">
+        <v>1</v>
+      </c>
+      <c r="E38" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="F38" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="13">
+        <v>95</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C39" s="13">
+        <v>1</v>
+      </c>
+      <c r="D39" s="13">
+        <v>1</v>
+      </c>
+      <c r="E39" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="F39" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="13">
+        <v>97.5</v>
+      </c>
+      <c r="B40" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C40" s="13">
+        <v>1</v>
+      </c>
+      <c r="D40" s="13">
+        <v>1</v>
+      </c>
+      <c r="E40" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="F40" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="13">
+        <v>100</v>
+      </c>
+      <c r="B41" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="C41" s="13">
+        <v>1</v>
+      </c>
+      <c r="D41" s="13">
+        <v>1</v>
+      </c>
+      <c r="E41" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="F41" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" s="13">
+        <v>102.5</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="C42" s="13">
+        <v>1</v>
+      </c>
+      <c r="D42" s="13">
+        <v>1</v>
+      </c>
+      <c r="E42" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="F42" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" s="13">
+        <v>105</v>
+      </c>
+      <c r="B43" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="C43" s="13">
+        <v>1</v>
+      </c>
+      <c r="D43" s="13">
+        <v>1</v>
+      </c>
+      <c r="E43" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="F43" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" s="13">
+        <v>107.5</v>
+      </c>
+      <c r="B44" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="C44" s="13">
+        <v>1</v>
+      </c>
+      <c r="D44" s="13">
+        <v>1</v>
+      </c>
+      <c r="E44" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="F44" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" s="13">
+        <v>110</v>
+      </c>
+      <c r="B45" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="C45" s="13">
+        <v>1</v>
+      </c>
+      <c r="D45" s="13">
+        <v>1</v>
+      </c>
+      <c r="E45" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="F45" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" s="13">
+        <v>112.5</v>
+      </c>
+      <c r="B46" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="C46" s="13">
+        <v>1</v>
+      </c>
+      <c r="D46" s="13">
+        <v>1</v>
+      </c>
+      <c r="E46" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="F46" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" s="13">
+        <v>115</v>
+      </c>
+      <c r="B47" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="C47" s="13">
+        <v>1</v>
+      </c>
+      <c r="D47" s="13">
+        <v>1</v>
+      </c>
+      <c r="E47" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="F47" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" s="13">
+        <v>117.5</v>
+      </c>
+      <c r="B48" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="C48" s="13">
+        <v>1</v>
+      </c>
+      <c r="D48" s="13">
+        <v>1</v>
+      </c>
+      <c r="E48" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="F48" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" s="13">
+        <v>120</v>
+      </c>
+      <c r="B49" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="C49" s="13">
+        <v>1</v>
+      </c>
+      <c r="D49" s="13">
+        <v>1</v>
+      </c>
+      <c r="E49" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="F49" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" s="13">
+        <v>122.5</v>
+      </c>
+      <c r="B50" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="C50" s="13">
+        <v>1</v>
+      </c>
+      <c r="D50" s="13">
+        <v>1</v>
+      </c>
+      <c r="E50" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="F50" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" s="13">
+        <v>125</v>
+      </c>
+      <c r="B51" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C51" s="13">
+        <v>1</v>
+      </c>
+      <c r="D51" s="13">
+        <v>1</v>
+      </c>
+      <c r="E51" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="F51" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" s="13">
+        <v>127.5</v>
+      </c>
+      <c r="B52" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="C52" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="D52" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="E52" s="13">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="F52" s="13">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" s="13">
+        <v>130</v>
+      </c>
+      <c r="B53" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="C53" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="D53" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="E53" s="13">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="F53" s="13">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" s="13">
+        <v>132.5</v>
+      </c>
+      <c r="B54" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="C54" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="D54" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="E54" s="13">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="F54" s="13">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" s="13">
+        <v>135</v>
+      </c>
+      <c r="B55" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="C55" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="D55" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="E55" s="13">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="F55" s="13">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" s="13">
+        <v>137.5</v>
+      </c>
+      <c r="B56" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="C56" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="D56" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="E56" s="13">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="F56" s="13">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57" s="13">
+        <v>140</v>
+      </c>
+      <c r="B57" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="C57" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="D57" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="E57" s="13">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="F57" s="13">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58" s="13">
+        <v>142.5</v>
+      </c>
+      <c r="B58" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="C58" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="D58" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="E58" s="13">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="F58" s="13">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59" s="13">
+        <v>145</v>
+      </c>
+      <c r="B59" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="C59" s="13">
+        <v>1</v>
+      </c>
+      <c r="D59" s="13">
+        <v>1</v>
+      </c>
+      <c r="E59" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="F59" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60" s="13">
+        <v>147.5</v>
+      </c>
+      <c r="B60" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="C60" s="13">
+        <v>1</v>
+      </c>
+      <c r="D60" s="13">
+        <v>1</v>
+      </c>
+      <c r="E60" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="F60" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61" s="13">
+        <v>150</v>
+      </c>
+      <c r="B61" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="C61" s="13">
+        <v>1</v>
+      </c>
+      <c r="D61" s="13">
+        <v>1</v>
+      </c>
+      <c r="E61" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="F61" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62" s="13">
+        <v>152.5</v>
+      </c>
+      <c r="B62" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="C62" s="13">
+        <v>1</v>
+      </c>
+      <c r="D62" s="13">
+        <v>1</v>
+      </c>
+      <c r="E62" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="F62" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63" s="13">
+        <v>155</v>
+      </c>
+      <c r="B63" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="C63" s="13">
+        <v>1</v>
+      </c>
+      <c r="D63" s="13">
+        <v>1</v>
+      </c>
+      <c r="E63" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="F63" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64" s="13">
+        <v>157.5</v>
+      </c>
+      <c r="B64" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="C64" s="13">
+        <v>1</v>
+      </c>
+      <c r="D64" s="13">
+        <v>1</v>
+      </c>
+      <c r="E64" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="F64" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
+      <c r="A65" s="13">
+        <v>160</v>
+      </c>
+      <c r="B65" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="C65" s="13">
+        <v>1</v>
+      </c>
+      <c r="D65" s="13">
+        <v>1</v>
+      </c>
+      <c r="E65" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="F65" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="A66" s="13">
+        <v>162.5</v>
+      </c>
+      <c r="B66" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="C66" s="13">
+        <v>1</v>
+      </c>
+      <c r="D66" s="13">
+        <v>1</v>
+      </c>
+      <c r="E66" s="13">
+        <f t="shared" ref="E66:F91" si="1">C66*1000</f>
+        <v>1000</v>
+      </c>
+      <c r="F66" s="13">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
+      <c r="A67" s="13">
+        <v>165</v>
+      </c>
+      <c r="B67" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C67" s="13">
+        <v>1</v>
+      </c>
+      <c r="D67" s="13">
+        <v>1</v>
+      </c>
+      <c r="E67" s="13">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+      <c r="F67" s="13">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
+      <c r="A68" s="13">
+        <v>167.5</v>
+      </c>
+      <c r="B68" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="C68" s="13">
+        <v>1</v>
+      </c>
+      <c r="D68" s="13">
+        <v>1</v>
+      </c>
+      <c r="E68" s="13">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+      <c r="F68" s="13">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
+      <c r="A69" s="13">
+        <v>170</v>
+      </c>
+      <c r="B69" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="C69" s="13">
+        <v>1</v>
+      </c>
+      <c r="D69" s="13">
+        <v>1</v>
+      </c>
+      <c r="E69" s="13">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+      <c r="F69" s="13">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
+      <c r="A70" s="13">
+        <v>172.5</v>
+      </c>
+      <c r="B70" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="C70" s="13">
+        <v>1</v>
+      </c>
+      <c r="D70" s="13">
+        <v>1</v>
+      </c>
+      <c r="E70" s="13">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+      <c r="F70" s="13">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
+      <c r="A71" s="13">
+        <v>175</v>
+      </c>
+      <c r="B71" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="C71" s="13">
+        <v>1</v>
+      </c>
+      <c r="D71" s="13">
+        <v>1</v>
+      </c>
+      <c r="E71" s="13">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+      <c r="F71" s="13">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
+      <c r="A72" s="13">
+        <v>177.5</v>
+      </c>
+      <c r="B72" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="C72" s="13">
+        <v>1</v>
+      </c>
+      <c r="D72" s="13">
+        <v>1</v>
+      </c>
+      <c r="E72" s="13">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+      <c r="F72" s="13">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6">
+      <c r="A73" s="13">
+        <v>180</v>
+      </c>
+      <c r="B73" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="C73" s="13">
+        <v>1</v>
+      </c>
+      <c r="D73" s="13">
+        <v>1</v>
+      </c>
+      <c r="E73" s="13">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+      <c r="F73" s="13">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6">
+      <c r="A74" s="13">
+        <v>182.5</v>
+      </c>
+      <c r="B74" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="C74" s="13">
+        <v>1</v>
+      </c>
+      <c r="D74" s="13">
+        <v>1</v>
+      </c>
+      <c r="E74" s="13">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+      <c r="F74" s="13">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6">
+      <c r="A75" s="13">
+        <v>185</v>
+      </c>
+      <c r="B75" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C75" s="13">
+        <v>1</v>
+      </c>
+      <c r="D75" s="13">
+        <v>1</v>
+      </c>
+      <c r="E75" s="13">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+      <c r="F75" s="13">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6">
+      <c r="A76" s="13">
+        <v>187.5</v>
+      </c>
+      <c r="B76" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="C76" s="13">
+        <v>1</v>
+      </c>
+      <c r="D76" s="13">
+        <v>1</v>
+      </c>
+      <c r="E76" s="13">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+      <c r="F76" s="13">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6">
+      <c r="A77" s="13">
+        <v>190</v>
+      </c>
+      <c r="B77" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="C77" s="13">
+        <v>1</v>
+      </c>
+      <c r="D77" s="13">
+        <v>1</v>
+      </c>
+      <c r="E77" s="13">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+      <c r="F77" s="13">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6">
+      <c r="A78" s="13">
+        <v>192.5</v>
+      </c>
+      <c r="B78" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="C78" s="13">
+        <v>1</v>
+      </c>
+      <c r="D78" s="13">
+        <v>1</v>
+      </c>
+      <c r="E78" s="13">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+      <c r="F78" s="13">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6">
+      <c r="A79" s="13">
+        <v>195</v>
+      </c>
+      <c r="B79" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="C79" s="13">
+        <v>1</v>
+      </c>
+      <c r="D79" s="13">
+        <v>1</v>
+      </c>
+      <c r="E79" s="13">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+      <c r="F79" s="13">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6">
+      <c r="A80" s="13">
+        <v>197.5</v>
+      </c>
+      <c r="B80" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="C80" s="13">
+        <v>1</v>
+      </c>
+      <c r="D80" s="13">
+        <v>1</v>
+      </c>
+      <c r="E80" s="13">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+      <c r="F80" s="13">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6">
+      <c r="A81" s="13">
+        <v>200</v>
+      </c>
+      <c r="B81" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="C81" s="13">
+        <v>1</v>
+      </c>
+      <c r="D81" s="13">
+        <v>1</v>
+      </c>
+      <c r="E81" s="13">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+      <c r="F81" s="13">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6">
+      <c r="A82" s="13">
+        <v>202.5</v>
+      </c>
+      <c r="B82" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="C82" s="13">
+        <v>1</v>
+      </c>
+      <c r="D82" s="13">
+        <v>1</v>
+      </c>
+      <c r="E82" s="13">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+      <c r="F82" s="13">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6">
+      <c r="A83" s="13">
+        <v>205</v>
+      </c>
+      <c r="B83" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="C83" s="13">
+        <v>1</v>
+      </c>
+      <c r="D83" s="13">
+        <v>1</v>
+      </c>
+      <c r="E83" s="13">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+      <c r="F83" s="13">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6">
+      <c r="A84" s="13">
+        <v>207.5</v>
+      </c>
+      <c r="B84" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="C84" s="13">
+        <v>1</v>
+      </c>
+      <c r="D84" s="13">
+        <v>1</v>
+      </c>
+      <c r="E84" s="13">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+      <c r="F84" s="13">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6">
+      <c r="A85" s="13">
+        <v>210</v>
+      </c>
+      <c r="B85" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="C85" s="13">
+        <v>1</v>
+      </c>
+      <c r="D85" s="13">
+        <v>1</v>
+      </c>
+      <c r="E85" s="13">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+      <c r="F85" s="13">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6">
+      <c r="A86" s="13">
+        <v>212.5</v>
+      </c>
+      <c r="B86" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="C86" s="13">
+        <v>1</v>
+      </c>
+      <c r="D86" s="13">
+        <v>1</v>
+      </c>
+      <c r="E86" s="13">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+      <c r="F86" s="13">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
+      <c r="A87" s="13">
+        <v>215</v>
+      </c>
+      <c r="B87" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C87" s="13">
+        <v>1</v>
+      </c>
+      <c r="D87" s="13">
+        <v>1</v>
+      </c>
+      <c r="E87" s="13">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+      <c r="F87" s="13">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6">
+      <c r="A88" s="13">
+        <v>217.5</v>
+      </c>
+      <c r="B88" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="C88" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="D88" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="E88" s="13">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="F88" s="13">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6">
+      <c r="A89" s="13">
+        <v>220</v>
+      </c>
+      <c r="B89" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="C89" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="D89" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="E89" s="13">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="F89" s="13">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6">
+      <c r="A90" s="13">
+        <v>222.5</v>
+      </c>
+      <c r="B90" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="C90" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="D90" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="E90" s="13">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="F90" s="13">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6">
+      <c r="A91" s="13">
+        <v>225</v>
+      </c>
+      <c r="B91" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="C91" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="D91" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="E91" s="13">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="F91" s="13">
+        <f t="shared" si="1"/>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Analysis 245: Harmonic power vs fundamental wave power
</commit_message>
<xml_diff>
--- a/245/data/Super_awesome_optical_freq_doubling.xlsx
+++ b/245/data/Super_awesome_optical_freq_doubling.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="19035" windowHeight="8445" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="19035" windowHeight="8445" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="75">
   <si>
     <t>Error</t>
   </si>
@@ -247,198 +247,6 @@
   <si>
     <t>lamba</t>
   </si>
-  <si>
-    <t>118.0 \pm 1.0</t>
-  </si>
-  <si>
-    <t>115.0 \pm 1.0</t>
-  </si>
-  <si>
-    <t>113.0 \pm 1.0</t>
-  </si>
-  <si>
-    <t>107.0 \pm 1.0</t>
-  </si>
-  <si>
-    <t>101.0 \pm 1.0</t>
-  </si>
-  <si>
-    <t>94.0 \pm 1.0</t>
-  </si>
-  <si>
-    <t>85.0 \pm 1.0</t>
-  </si>
-  <si>
-    <t>75.0 \pm 1.0</t>
-  </si>
-  <si>
-    <t>65.0 \pm 1.0</t>
-  </si>
-  <si>
-    <t>55.0 \pm 1.0</t>
-  </si>
-  <si>
-    <t>46.0 \pm 1.0</t>
-  </si>
-  <si>
-    <t>36.0 \pm 1.0</t>
-  </si>
-  <si>
-    <t>26.0 \pm 1.0</t>
-  </si>
-  <si>
-    <t>20.0 \pm 1.0</t>
-  </si>
-  <si>
-    <t>13.0 \pm 1.0</t>
-  </si>
-  <si>
-    <t>7.0 \pm 0.1</t>
-  </si>
-  <si>
-    <t>3.0 \pm 0.1</t>
-  </si>
-  <si>
-    <t>0.8 \pm 0.1</t>
-  </si>
-  <si>
-    <t>0.3 \pm 0.1</t>
-  </si>
-  <si>
-    <t>1.5 \pm 0.1</t>
-  </si>
-  <si>
-    <t>4.8 \pm 0.1</t>
-  </si>
-  <si>
-    <t>8.8 \pm 0.1</t>
-  </si>
-  <si>
-    <t>16.0 \pm 1.0</t>
-  </si>
-  <si>
-    <t>23.0 \pm 1.0</t>
-  </si>
-  <si>
-    <t>32.0 \pm 1.0</t>
-  </si>
-  <si>
-    <t>41.0 \pm 1.0</t>
-  </si>
-  <si>
-    <t>51.0 \pm 1.0</t>
-  </si>
-  <si>
-    <t>61.0 \pm 1.0</t>
-  </si>
-  <si>
-    <t>72.0 \pm 1.0</t>
-  </si>
-  <si>
-    <t>80.0 \pm 1.0</t>
-  </si>
-  <si>
-    <t>90.0 \pm 1.0</t>
-  </si>
-  <si>
-    <t>97.0 \pm 1.0</t>
-  </si>
-  <si>
-    <t>105.0 \pm 1.0</t>
-  </si>
-  <si>
-    <t>110.0 \pm 1.0</t>
-  </si>
-  <si>
-    <t>117.0 \pm 1.0</t>
-  </si>
-  <si>
-    <t>116.0 \pm 1.0</t>
-  </si>
-  <si>
-    <t>109.0 \pm 1.0</t>
-  </si>
-  <si>
-    <t>102.0 \pm 1.0</t>
-  </si>
-  <si>
-    <t>95.0 \pm 1.0</t>
-  </si>
-  <si>
-    <t>87.0 \pm 1.0</t>
-  </si>
-  <si>
-    <t>78.0 \pm 1.0</t>
-  </si>
-  <si>
-    <t>67.0 \pm 1.0</t>
-  </si>
-  <si>
-    <t>58.0 \pm 1.0</t>
-  </si>
-  <si>
-    <t>39.0 \pm 1.0</t>
-  </si>
-  <si>
-    <t>28.0 \pm 1.0</t>
-  </si>
-  <si>
-    <t>21.0 \pm 1.0</t>
-  </si>
-  <si>
-    <t>8.0 \pm 0.1</t>
-  </si>
-  <si>
-    <t>4.0 \pm 0.1</t>
-  </si>
-  <si>
-    <t>2.0 \pm 0.1</t>
-  </si>
-  <si>
-    <t>1.9 \pm 0.1</t>
-  </si>
-  <si>
-    <t>5.0 \pm 0.1</t>
-  </si>
-  <si>
-    <t>9.0 \pm 0.1</t>
-  </si>
-  <si>
-    <t>22.0 \pm 1.0</t>
-  </si>
-  <si>
-    <t>31.0 \pm 1.0</t>
-  </si>
-  <si>
-    <t>40.0 \pm 1.0</t>
-  </si>
-  <si>
-    <t>50.0 \pm 1.0</t>
-  </si>
-  <si>
-    <t>60.0 \pm 1.0</t>
-  </si>
-  <si>
-    <t>71.0 \pm 1.0</t>
-  </si>
-  <si>
-    <t>106.0 \pm 1.0</t>
-  </si>
-  <si>
-    <t>111.0 \pm 1.0</t>
-  </si>
-  <si>
-    <t>96.0 \pm 1.0</t>
-  </si>
-  <si>
-    <t>86.0 \pm 1.0</t>
-  </si>
-  <si>
-    <t>1.0 \pm 0.1</t>
-  </si>
-  <si>
-    <t>0.4 \pm 0.1</t>
-  </si>
 </sst>
 </file>
 
@@ -517,7 +325,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -532,6 +340,7 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -871,8 +680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q53"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1747,8 +1556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K98"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -3992,7 +3801,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -4020,7 +3829,7 @@
   <dimension ref="A1:K70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -5725,10 +5534,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N81"/>
+  <dimension ref="A1:S81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="A7" sqref="A7:I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -5737,22 +5546,26 @@
     <col min="3" max="3" width="20" customWidth="1"/>
     <col min="8" max="8" width="17.85546875" customWidth="1"/>
     <col min="12" max="12" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:19">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:19">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:19">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:19">
       <c r="K4" s="1" t="s">
         <v>65</v>
       </c>
@@ -5760,7 +5573,7 @@
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
     </row>
-    <row r="5" spans="1:14" s="2" customFormat="1">
+    <row r="5" spans="1:19" s="2" customFormat="1">
       <c r="A5" s="2" t="s">
         <v>62</v>
       </c>
@@ -5795,7 +5608,7 @@
       <c r="M5"/>
       <c r="N5"/>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:19">
       <c r="A7">
         <v>0</v>
       </c>
@@ -5833,8 +5646,12 @@
       <c r="M7" s="8" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="8" spans="1:14">
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+    </row>
+    <row r="8" spans="1:19">
       <c r="A8">
         <v>2.5</v>
       </c>
@@ -5878,8 +5695,12 @@
       <c r="N8" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="9" spans="1:14">
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+    </row>
+    <row r="9" spans="1:19">
       <c r="A9">
         <v>5</v>
       </c>
@@ -5920,8 +5741,12 @@
       <c r="M9" s="7">
         <v>1.323E-5</v>
       </c>
-    </row>
-    <row r="10" spans="1:14">
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+    </row>
+    <row r="10" spans="1:19">
       <c r="A10">
         <v>7.5</v>
       </c>
@@ -5953,8 +5778,12 @@
         <f t="shared" si="3"/>
         <v>2.0045938492086832</v>
       </c>
-    </row>
-    <row r="11" spans="1:14">
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+      <c r="S10" s="3"/>
+    </row>
+    <row r="11" spans="1:19">
       <c r="A11">
         <v>10</v>
       </c>
@@ -5986,8 +5815,12 @@
         <f t="shared" si="3"/>
         <v>2.5582646947136163</v>
       </c>
-    </row>
-    <row r="12" spans="1:14">
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="3"/>
+    </row>
+    <row r="12" spans="1:19">
       <c r="A12">
         <v>12.5</v>
       </c>
@@ -6019,8 +5852,12 @@
         <f t="shared" si="3"/>
         <v>3.037954364508034</v>
       </c>
-    </row>
-    <row r="13" spans="1:14">
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
+      <c r="S12" s="3"/>
+    </row>
+    <row r="13" spans="1:19">
       <c r="A13">
         <v>15</v>
       </c>
@@ -6052,8 +5889,12 @@
         <f t="shared" si="3"/>
         <v>3.4271936217363717</v>
       </c>
-    </row>
-    <row r="14" spans="1:14">
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
+      <c r="S13" s="3"/>
+    </row>
+    <row r="14" spans="1:19">
       <c r="A14">
         <v>17.5</v>
       </c>
@@ -6088,8 +5929,12 @@
       <c r="K14" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="15" spans="1:14">
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
+      <c r="S14" s="3"/>
+    </row>
+    <row r="15" spans="1:19">
       <c r="A15">
         <v>20</v>
       </c>
@@ -6124,8 +5969,12 @@
       <c r="K15" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="16" spans="1:14">
+      <c r="P15" s="3"/>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="3"/>
+      <c r="S15" s="3"/>
+    </row>
+    <row r="16" spans="1:19">
       <c r="A16">
         <v>22.5</v>
       </c>
@@ -6157,8 +6006,12 @@
         <f t="shared" si="3"/>
         <v>3.9427695282759787</v>
       </c>
-    </row>
-    <row r="17" spans="1:13">
+      <c r="P16" s="3"/>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="3"/>
+      <c r="S16" s="3"/>
+    </row>
+    <row r="17" spans="1:19">
       <c r="A17">
         <v>25</v>
       </c>
@@ -6196,8 +6049,12 @@
       <c r="M17" s="8" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="18" spans="1:13">
+      <c r="P17" s="3"/>
+      <c r="Q17" s="3"/>
+      <c r="R17" s="3"/>
+      <c r="S17" s="3"/>
+    </row>
+    <row r="18" spans="1:19">
       <c r="A18">
         <v>27.5</v>
       </c>
@@ -6238,8 +6095,12 @@
       <c r="M18" s="11">
         <v>1.9619999999999998E-5</v>
       </c>
-    </row>
-    <row r="19" spans="1:13">
+      <c r="P18" s="3"/>
+      <c r="Q18" s="3"/>
+      <c r="R18" s="3"/>
+      <c r="S18" s="3"/>
+    </row>
+    <row r="19" spans="1:19">
       <c r="A19">
         <v>30</v>
       </c>
@@ -6271,8 +6132,12 @@
         <f t="shared" si="3"/>
         <v>3.4022346269051393</v>
       </c>
-    </row>
-    <row r="20" spans="1:13">
+      <c r="P19" s="3"/>
+      <c r="Q19" s="3"/>
+      <c r="R19" s="3"/>
+      <c r="S19" s="3"/>
+    </row>
+    <row r="20" spans="1:19">
       <c r="A20">
         <v>32.5</v>
       </c>
@@ -6304,8 +6169,12 @@
         <f t="shared" si="3"/>
         <v>3.0041138395583999</v>
       </c>
-    </row>
-    <row r="21" spans="1:13">
+      <c r="P20" s="3"/>
+      <c r="Q20" s="3"/>
+      <c r="R20" s="3"/>
+      <c r="S20" s="3"/>
+    </row>
+    <row r="21" spans="1:19">
       <c r="A21">
         <v>35</v>
       </c>
@@ -6337,8 +6206,12 @@
         <f t="shared" si="3"/>
         <v>2.5144818402151099</v>
       </c>
-    </row>
-    <row r="22" spans="1:13">
+      <c r="P21" s="3"/>
+      <c r="Q21" s="3"/>
+      <c r="R21" s="3"/>
+      <c r="S21" s="3"/>
+    </row>
+    <row r="22" spans="1:19">
       <c r="A22">
         <v>37.5</v>
       </c>
@@ -6370,8 +6243,12 @@
         <f t="shared" si="3"/>
         <v>1.948232931073471</v>
       </c>
-    </row>
-    <row r="23" spans="1:13">
+      <c r="P22" s="3"/>
+      <c r="Q22" s="3"/>
+      <c r="R22" s="3"/>
+      <c r="S22" s="3"/>
+    </row>
+    <row r="23" spans="1:19">
       <c r="A23">
         <v>40</v>
       </c>
@@ -6403,8 +6280,12 @@
         <f t="shared" si="3"/>
         <v>1.322606436529951</v>
       </c>
-    </row>
-    <row r="24" spans="1:13">
+      <c r="P23" s="3"/>
+      <c r="Q23" s="3"/>
+      <c r="R23" s="3"/>
+      <c r="S23" s="3"/>
+    </row>
+    <row r="24" spans="1:19">
       <c r="A24">
         <v>42.5</v>
       </c>
@@ -6436,8 +6317,12 @@
         <f t="shared" si="3"/>
         <v>0.65665852544455006</v>
       </c>
-    </row>
-    <row r="25" spans="1:13">
+      <c r="P24" s="3"/>
+      <c r="Q24" s="3"/>
+      <c r="R24" s="3"/>
+      <c r="S24" s="3"/>
+    </row>
+    <row r="25" spans="1:19">
       <c r="A25">
         <v>45</v>
       </c>
@@ -6469,8 +6354,12 @@
         <f t="shared" si="3"/>
         <v>2.9320931119283793E-2</v>
       </c>
-    </row>
-    <row r="26" spans="1:13">
+      <c r="P25" s="3"/>
+      <c r="Q25" s="3"/>
+      <c r="R25" s="3"/>
+      <c r="S25" s="3"/>
+    </row>
+    <row r="26" spans="1:19">
       <c r="A26">
         <v>47.5</v>
       </c>
@@ -6502,8 +6391,12 @@
         <f t="shared" si="3"/>
         <v>0.71442889299342249</v>
       </c>
-    </row>
-    <row r="27" spans="1:13">
+      <c r="P26" s="3"/>
+      <c r="Q26" s="3"/>
+      <c r="R26" s="3"/>
+      <c r="S26" s="3"/>
+    </row>
+    <row r="27" spans="1:19">
       <c r="A27">
         <v>50</v>
       </c>
@@ -6535,8 +6428,12 @@
         <f t="shared" si="3"/>
         <v>1.3777882938644588</v>
       </c>
-    </row>
-    <row r="28" spans="1:13">
+      <c r="P27" s="3"/>
+      <c r="Q27" s="3"/>
+      <c r="R27" s="3"/>
+      <c r="S27" s="3"/>
+    </row>
+    <row r="28" spans="1:19">
       <c r="A28">
         <v>52.5</v>
       </c>
@@ -6568,8 +6465,12 @@
         <f t="shared" si="3"/>
         <v>1.9991864173081153</v>
       </c>
-    </row>
-    <row r="29" spans="1:13">
+      <c r="P28" s="3"/>
+      <c r="Q28" s="3"/>
+      <c r="R28" s="3"/>
+      <c r="S28" s="3"/>
+    </row>
+    <row r="29" spans="1:19">
       <c r="A29">
         <v>55</v>
       </c>
@@ -6601,8 +6502,12 @@
         <f t="shared" si="3"/>
         <v>2.5596931530233067</v>
       </c>
-    </row>
-    <row r="30" spans="1:13">
+      <c r="P29" s="3"/>
+      <c r="Q29" s="3"/>
+      <c r="R29" s="3"/>
+      <c r="S29" s="3"/>
+    </row>
+    <row r="30" spans="1:19">
       <c r="A30">
         <v>57.5</v>
       </c>
@@ -6634,8 +6539,12 @@
         <f t="shared" si="3"/>
         <v>3.0422404237141905</v>
       </c>
-    </row>
-    <row r="31" spans="1:13">
+      <c r="P30" s="3"/>
+      <c r="Q30" s="3"/>
+      <c r="R30" s="3"/>
+      <c r="S30" s="3"/>
+    </row>
+    <row r="31" spans="1:19">
       <c r="A31">
         <v>60</v>
       </c>
@@ -6667,8 +6576,12 @@
         <f t="shared" si="3"/>
         <v>3.4321453271878202</v>
       </c>
-    </row>
-    <row r="32" spans="1:13">
+      <c r="P31" s="3"/>
+      <c r="Q31" s="3"/>
+      <c r="R31" s="3"/>
+      <c r="S31" s="3"/>
+    </row>
+    <row r="32" spans="1:19">
       <c r="A32">
         <v>62.5</v>
       </c>
@@ -6700,8 +6613,12 @@
         <f t="shared" si="3"/>
         <v>3.7175613925695852</v>
       </c>
-    </row>
-    <row r="33" spans="1:9">
+      <c r="P32" s="3"/>
+      <c r="Q32" s="3"/>
+      <c r="R32" s="3"/>
+      <c r="S32" s="3"/>
+    </row>
+    <row r="33" spans="1:19">
       <c r="A33">
         <v>65</v>
       </c>
@@ -6733,8 +6650,12 @@
         <f t="shared" si="3"/>
         <v>3.8898448086638835</v>
       </c>
-    </row>
-    <row r="34" spans="1:9">
+      <c r="P33" s="3"/>
+      <c r="Q33" s="3"/>
+      <c r="R33" s="3"/>
+      <c r="S33" s="3"/>
+    </row>
+    <row r="34" spans="1:19">
       <c r="A34">
         <v>67.5</v>
       </c>
@@ -6766,8 +6687,12 @@
         <f t="shared" si="3"/>
         <v>3.9438256083629719</v>
       </c>
-    </row>
-    <row r="35" spans="1:9">
+      <c r="P34" s="3"/>
+      <c r="Q34" s="3"/>
+      <c r="R34" s="3"/>
+      <c r="S34" s="3"/>
+    </row>
+    <row r="35" spans="1:19">
       <c r="A35">
         <v>70</v>
       </c>
@@ -6799,8 +6724,12 @@
         <f t="shared" si="3"/>
         <v>3.8779778145166532</v>
       </c>
-    </row>
-    <row r="36" spans="1:9">
+      <c r="P35" s="3"/>
+      <c r="Q35" s="3"/>
+      <c r="R35" s="3"/>
+      <c r="S35" s="3"/>
+    </row>
+    <row r="36" spans="1:19">
       <c r="A36">
         <v>72.5</v>
       </c>
@@ -6832,8 +6761,12 @@
         <f t="shared" si="3"/>
         <v>3.6944881755525207</v>
       </c>
-    </row>
-    <row r="37" spans="1:9">
+      <c r="P36" s="3"/>
+      <c r="Q36" s="3"/>
+      <c r="R36" s="3"/>
+      <c r="S36" s="3"/>
+    </row>
+    <row r="37" spans="1:19">
       <c r="A37">
         <v>75</v>
       </c>
@@ -6865,8 +6798,12 @@
         <f t="shared" si="3"/>
         <v>3.399232501308628</v>
       </c>
-    </row>
-    <row r="38" spans="1:9">
+      <c r="P37" s="3"/>
+      <c r="Q37" s="3"/>
+      <c r="R37" s="3"/>
+      <c r="S37" s="3"/>
+    </row>
+    <row r="38" spans="1:19">
       <c r="A38">
         <v>77.5</v>
       </c>
@@ -6898,8 +6835,12 @@
         <f t="shared" si="3"/>
         <v>3.00168885330593</v>
       </c>
-    </row>
-    <row r="39" spans="1:9">
+      <c r="P38" s="3"/>
+      <c r="Q38" s="3"/>
+      <c r="R38" s="3"/>
+      <c r="S38" s="3"/>
+    </row>
+    <row r="39" spans="1:19">
       <c r="A39">
         <v>80</v>
       </c>
@@ -6931,8 +6872,12 @@
         <f t="shared" si="3"/>
         <v>2.5148747145630668</v>
       </c>
-    </row>
-    <row r="40" spans="1:9">
+      <c r="P39" s="3"/>
+      <c r="Q39" s="3"/>
+      <c r="R39" s="3"/>
+      <c r="S39" s="3"/>
+    </row>
+    <row r="40" spans="1:19">
       <c r="A40">
         <v>82.5</v>
       </c>
@@ -6964,8 +6909,12 @@
         <f t="shared" si="3"/>
         <v>1.9556143558971697</v>
       </c>
-    </row>
-    <row r="41" spans="1:9">
+      <c r="P40" s="3"/>
+      <c r="Q40" s="3"/>
+      <c r="R40" s="3"/>
+      <c r="S40" s="3"/>
+    </row>
+    <row r="41" spans="1:19">
       <c r="A41">
         <v>85</v>
       </c>
@@ -6997,8 +6946,12 @@
         <f t="shared" si="3"/>
         <v>1.346597798918223</v>
       </c>
-    </row>
-    <row r="42" spans="1:9">
+      <c r="P41" s="3"/>
+      <c r="Q41" s="3"/>
+      <c r="R41" s="3"/>
+      <c r="S41" s="3"/>
+    </row>
+    <row r="42" spans="1:19">
       <c r="A42">
         <v>87.5</v>
       </c>
@@ -7030,8 +6983,12 @@
         <f t="shared" si="3"/>
         <v>0.73183388137707039</v>
       </c>
-    </row>
-    <row r="43" spans="1:9">
+      <c r="P42" s="3"/>
+      <c r="Q42" s="3"/>
+      <c r="R42" s="3"/>
+      <c r="S42" s="3"/>
+    </row>
+    <row r="43" spans="1:19">
       <c r="A43">
         <v>90</v>
       </c>
@@ -7063,8 +7020,12 @@
         <f t="shared" si="3"/>
         <v>0.38270229986474558</v>
       </c>
-    </row>
-    <row r="44" spans="1:9">
+      <c r="P43" s="3"/>
+      <c r="Q43" s="3"/>
+      <c r="R43" s="3"/>
+      <c r="S43" s="3"/>
+    </row>
+    <row r="44" spans="1:19">
       <c r="A44">
         <v>92.5</v>
       </c>
@@ -7096,8 +7057,12 @@
         <f t="shared" si="3"/>
         <v>0.83269216227488452</v>
       </c>
-    </row>
-    <row r="45" spans="1:9">
+      <c r="P44" s="3"/>
+      <c r="Q44" s="3"/>
+      <c r="R44" s="3"/>
+      <c r="S44" s="3"/>
+    </row>
+    <row r="45" spans="1:19">
       <c r="A45">
         <v>95</v>
       </c>
@@ -7129,8 +7094,12 @@
         <f t="shared" si="3"/>
         <v>1.452624218754506</v>
       </c>
-    </row>
-    <row r="46" spans="1:9">
+      <c r="P45" s="3"/>
+      <c r="Q45" s="3"/>
+      <c r="R45" s="3"/>
+      <c r="S45" s="3"/>
+    </row>
+    <row r="46" spans="1:19">
       <c r="A46">
         <v>97.5</v>
       </c>
@@ -7163,7 +7132,7 @@
         <v>2.0554481128725173</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:19">
       <c r="A47">
         <v>100</v>
       </c>
@@ -7196,7 +7165,7 @@
         <v>2.6040386009568768</v>
       </c>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:19">
       <c r="A48">
         <v>102.5</v>
       </c>
@@ -10535,2019 +10504,680 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F91"/>
+  <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="4" width="11.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" style="13"/>
+    <col min="1" max="1" width="11.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="11.42578125" style="13"/>
+    <col min="5" max="6" width="11.5703125" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="13">
+      <c r="A1">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
-        <v>75</v>
+      <c r="B1" s="13">
+        <v>112.553</v>
       </c>
       <c r="C1" s="13">
-        <v>1</v>
-      </c>
-      <c r="D1" s="13">
-        <v>1</v>
-      </c>
-      <c r="E1" s="13">
-        <f>C1*1000</f>
-        <v>1000</v>
-      </c>
-      <c r="F1" s="13">
-        <f>D1*1000</f>
-        <v>1000</v>
+        <v>0.37819999999999998</v>
+      </c>
+      <c r="D1">
+        <v>23.7</v>
+      </c>
+      <c r="E1">
+        <v>0.01</v>
+      </c>
+      <c r="F1">
+        <v>0.1</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="13">
+      <c r="A2">
         <v>2.5</v>
       </c>
-      <c r="B2" s="13" t="s">
-        <v>76</v>
+      <c r="B2" s="13">
+        <v>111.693987190893</v>
       </c>
       <c r="C2" s="13">
-        <v>1</v>
-      </c>
-      <c r="D2" s="13">
-        <v>1</v>
-      </c>
-      <c r="E2" s="13">
-        <f t="shared" ref="E2:F65" si="0">C2*1000</f>
-        <v>1000</v>
-      </c>
-      <c r="F2" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
+        <v>0.78148028788541435</v>
+      </c>
+      <c r="D2">
+        <v>23</v>
+      </c>
+      <c r="E2">
+        <v>0.01</v>
+      </c>
+      <c r="F2">
+        <v>0.1</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="13">
+      <c r="A3">
         <v>5</v>
       </c>
-      <c r="B3" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="C3" s="13">
-        <v>1</v>
-      </c>
-      <c r="D3" s="13">
-        <v>1</v>
-      </c>
-      <c r="E3" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="F3" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
+      <c r="B3" s="14">
+        <v>109.1431729603935</v>
+      </c>
+      <c r="C3" s="14">
+        <v>1.3989182962915241</v>
+      </c>
+      <c r="D3">
+        <v>21.4</v>
+      </c>
+      <c r="E3">
+        <v>0.01</v>
+      </c>
+      <c r="F3">
+        <v>0.1</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="13">
+      <c r="A4">
         <v>7.5</v>
       </c>
-      <c r="B4" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="C4" s="13">
-        <v>1</v>
-      </c>
-      <c r="D4" s="13">
-        <v>1</v>
-      </c>
-      <c r="E4" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="F4" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
+      <c r="B4" s="14">
+        <v>104.9784293189374</v>
+      </c>
+      <c r="C4" s="14">
+        <v>2.0045938492086832</v>
+      </c>
+      <c r="D4">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="E4">
+        <v>0.01</v>
+      </c>
+      <c r="F4">
+        <v>0.1</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="13">
+      <c r="A5">
         <v>10</v>
       </c>
-      <c r="B5" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="C5" s="13">
-        <v>1</v>
-      </c>
-      <c r="D5" s="13">
-        <v>1</v>
-      </c>
-      <c r="E5" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="F5" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
+      <c r="B5" s="14">
+        <v>99.32689879083452</v>
+      </c>
+      <c r="C5" s="14">
+        <v>2.5582646947136163</v>
+      </c>
+      <c r="D5">
+        <v>17.5</v>
+      </c>
+      <c r="E5">
+        <v>0.01</v>
+      </c>
+      <c r="F5">
+        <v>0.1</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="13">
+      <c r="A6">
         <v>12.5</v>
       </c>
-      <c r="B6" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="C6" s="13">
-        <v>1</v>
-      </c>
-      <c r="D6" s="13">
-        <v>1</v>
-      </c>
-      <c r="E6" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="F6" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
+      <c r="B6" s="14">
+        <v>92.361112969723337</v>
+      </c>
+      <c r="C6" s="14">
+        <v>3.037954364508034</v>
+      </c>
+      <c r="D6">
+        <v>15.3</v>
+      </c>
+      <c r="E6">
+        <v>0.01</v>
+      </c>
+      <c r="F6">
+        <v>0.1</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="13">
+      <c r="A7">
         <v>15</v>
       </c>
-      <c r="B7" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="C7" s="13">
-        <v>1</v>
-      </c>
-      <c r="D7" s="13">
-        <v>1</v>
-      </c>
-      <c r="E7" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="F7" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
+      <c r="B7" s="14">
+        <v>84.293725423108256</v>
+      </c>
+      <c r="C7" s="14">
+        <v>3.4271936217363717</v>
+      </c>
+      <c r="D7">
+        <v>12.6</v>
+      </c>
+      <c r="E7">
+        <v>0.01</v>
+      </c>
+      <c r="F7">
+        <v>0.1</v>
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="13">
+      <c r="A8">
         <v>17.5</v>
       </c>
-      <c r="B8" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="C8" s="13">
-        <v>1</v>
-      </c>
-      <c r="D8" s="13">
-        <v>1</v>
-      </c>
-      <c r="E8" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="F8" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
+      <c r="B8" s="14">
+        <v>75.371019741424803</v>
+      </c>
+      <c r="C8" s="14">
+        <v>3.7132629587734853</v>
+      </c>
+      <c r="D8">
+        <v>9.9</v>
+      </c>
+      <c r="E8">
+        <v>0.01</v>
+      </c>
+      <c r="F8">
+        <v>0.01</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="13">
+      <c r="A9">
         <v>20</v>
       </c>
-      <c r="B9" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="C9" s="13">
-        <v>1</v>
-      </c>
-      <c r="D9" s="13">
-        <v>1</v>
-      </c>
-      <c r="E9" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="F9" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
+      <c r="B9" s="14">
+        <v>65.865390919829281</v>
+      </c>
+      <c r="C9" s="14">
+        <v>3.8869796423982366</v>
+      </c>
+      <c r="D9">
+        <v>7</v>
+      </c>
+      <c r="E9">
+        <v>0.01</v>
+      </c>
+      <c r="F9">
+        <v>0.01</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="13">
+      <c r="A10">
         <v>22.5</v>
       </c>
-      <c r="B10" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="C10" s="13">
-        <v>1</v>
-      </c>
-      <c r="D10" s="13">
-        <v>1</v>
-      </c>
-      <c r="E10" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="F10" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
+      <c r="B10" s="14">
+        <v>56.067029603310949</v>
+      </c>
+      <c r="C10" s="14">
+        <v>3.9427695282759787</v>
+      </c>
+      <c r="D10">
+        <v>5.2</v>
+      </c>
+      <c r="E10">
+        <v>0.01</v>
+      </c>
+      <c r="F10">
+        <v>0.01</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="13">
+      <c r="A11">
         <v>25</v>
       </c>
-      <c r="B11" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="C11" s="13">
-        <v>1</v>
-      </c>
-      <c r="D11" s="13">
-        <v>1</v>
-      </c>
-      <c r="E11" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="F11" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
+      <c r="B11" s="14">
+        <v>46.27506306094822</v>
+      </c>
+      <c r="C11" s="14">
+        <v>3.8787510651947663</v>
+      </c>
+      <c r="D11">
+        <v>3.5</v>
+      </c>
+      <c r="E11">
+        <v>0.01</v>
+      </c>
+      <c r="F11">
+        <v>0.01</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="13">
+      <c r="A12">
         <v>27.5</v>
       </c>
-      <c r="B12" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="C12" s="13">
-        <v>1</v>
-      </c>
-      <c r="D12" s="13">
-        <v>1</v>
-      </c>
-      <c r="E12" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="F12" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
+      <c r="B12" s="14">
+        <v>36.788423340264913</v>
+      </c>
+      <c r="C12" s="14">
+        <v>3.696752369519364</v>
+      </c>
+      <c r="D12">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E12">
+        <v>0.01</v>
+      </c>
+      <c r="F12">
+        <v>0.01</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="13">
+      <c r="A13">
         <v>30</v>
       </c>
-      <c r="B13" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="C13" s="13">
-        <v>1</v>
-      </c>
-      <c r="D13" s="13">
-        <v>1</v>
-      </c>
-      <c r="E13" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="F13" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
+      <c r="B13" s="14">
+        <v>27.896721381367488</v>
+      </c>
+      <c r="C13" s="14">
+        <v>3.4022346269051393</v>
+      </c>
+      <c r="D13">
+        <v>1.3</v>
+      </c>
+      <c r="E13">
+        <v>0.01</v>
+      </c>
+      <c r="F13">
+        <v>0.01</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="13">
+      <c r="A14">
         <v>32.5</v>
       </c>
-      <c r="B14" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="C14" s="13">
-        <v>1</v>
-      </c>
-      <c r="D14" s="13">
-        <v>1</v>
-      </c>
-      <c r="E14" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="F14" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
+      <c r="B14" s="14">
+        <v>19.871405688603378</v>
+      </c>
+      <c r="C14" s="14">
+        <v>3.0041138395583999</v>
+      </c>
+      <c r="D14">
+        <v>0.8</v>
+      </c>
+      <c r="E14">
+        <v>0.01</v>
+      </c>
+      <c r="F14">
+        <v>0.01</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="13">
+      <c r="A15">
         <v>35</v>
       </c>
-      <c r="B15" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="C15" s="13">
-        <v>1</v>
-      </c>
-      <c r="D15" s="13">
-        <v>1</v>
-      </c>
-      <c r="E15" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="F15" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
+      <c r="B15" s="14">
+        <v>12.957475470424107</v>
+      </c>
+      <c r="C15" s="14">
+        <v>2.5144818402151099</v>
+      </c>
+      <c r="D15">
+        <v>0.4</v>
+      </c>
+      <c r="E15">
+        <v>0.01</v>
+      </c>
+      <c r="F15">
+        <v>0.01</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="13">
+      <c r="A16">
         <v>37.5</v>
       </c>
-      <c r="B16" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="C16" s="13">
-        <v>0.1</v>
-      </c>
-      <c r="D16" s="13">
-        <v>0.1</v>
-      </c>
-      <c r="E16" s="13">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="F16" s="13">
-        <f t="shared" si="0"/>
-        <v>100</v>
+      <c r="B16" s="14">
+        <v>7.3660012311676759</v>
+      </c>
+      <c r="C16" s="14">
+        <v>1.948232931073471</v>
+      </c>
+      <c r="D16">
+        <v>0.2</v>
+      </c>
+      <c r="E16">
+        <v>0.01</v>
+      </c>
+      <c r="F16">
+        <v>0.01</v>
       </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="13">
+      <c r="A17">
         <v>40</v>
       </c>
-      <c r="B17" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="C17" s="13">
-        <v>0.1</v>
-      </c>
-      <c r="D17" s="13">
-        <v>0.1</v>
-      </c>
-      <c r="E17" s="13">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="F17" s="13">
-        <f t="shared" si="0"/>
-        <v>100</v>
+      <c r="B17" s="14">
+        <v>3.2676811483437938</v>
+      </c>
+      <c r="C17" s="14">
+        <v>1.322606436529951</v>
+      </c>
+      <c r="D17">
+        <v>0.11</v>
+      </c>
+      <c r="E17">
+        <v>0.01</v>
+      </c>
+      <c r="F17">
+        <v>0.01</v>
       </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="13">
+      <c r="A18">
         <v>42.5</v>
       </c>
-      <c r="B18" s="13" t="s">
-        <v>92</v>
+      <c r="B18" s="13">
+        <v>0.78762994824019816</v>
       </c>
       <c r="C18" s="13">
-        <v>0.1</v>
-      </c>
-      <c r="D18" s="13">
-        <v>0.1</v>
-      </c>
-      <c r="E18" s="13">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="F18" s="13">
-        <f t="shared" si="0"/>
-        <v>100</v>
+        <v>0.65665852544455006</v>
+      </c>
+      <c r="D18">
+        <v>0.09</v>
+      </c>
+      <c r="E18">
+        <v>0.01</v>
+      </c>
+      <c r="F18">
+        <v>0.01</v>
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="13">
+      <c r="A19">
         <v>45</v>
       </c>
-      <c r="B19" s="13" t="s">
-        <v>93</v>
+      <c r="B19" s="13">
+        <v>1.5593665949043955E-3</v>
       </c>
       <c r="C19" s="13">
-        <v>0.1</v>
-      </c>
-      <c r="D19" s="13">
-        <v>0.1</v>
-      </c>
-      <c r="E19" s="13">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="F19" s="13">
-        <f t="shared" si="0"/>
-        <v>100</v>
+        <v>2.9320931119283793E-2</v>
+      </c>
+      <c r="D19">
+        <v>0.09</v>
+      </c>
+      <c r="E19">
+        <v>0.01</v>
+      </c>
+      <c r="F19">
+        <v>0.01</v>
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="13">
-        <v>47.5</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="C20" s="13">
-        <v>0.1</v>
-      </c>
-      <c r="D20" s="13">
-        <v>0.1</v>
-      </c>
-      <c r="E20" s="13">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="F20" s="13">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
+      <c r="A20"/>
+      <c r="D20"/>
+      <c r="E20"/>
+      <c r="F20"/>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="13">
-        <v>50</v>
-      </c>
-      <c r="B21" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="C21" s="13">
-        <v>0.1</v>
-      </c>
-      <c r="D21" s="13">
-        <v>0.1</v>
-      </c>
-      <c r="E21" s="13">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="F21" s="13">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
+      <c r="A21"/>
+      <c r="D21"/>
+      <c r="E21"/>
+      <c r="F21"/>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="13">
-        <v>52.5</v>
-      </c>
-      <c r="B22" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="C22" s="13">
-        <v>0.1</v>
-      </c>
-      <c r="D22" s="13">
-        <v>0.1</v>
-      </c>
-      <c r="E22" s="13">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="F22" s="13">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
+      <c r="A22"/>
+      <c r="D22"/>
+      <c r="E22"/>
+      <c r="F22"/>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="13">
-        <v>55</v>
-      </c>
-      <c r="B23" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="C23" s="13">
-        <v>1</v>
-      </c>
-      <c r="D23" s="13">
-        <v>1</v>
-      </c>
-      <c r="E23" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="F23" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
+      <c r="A23"/>
+      <c r="D23"/>
+      <c r="E23"/>
+      <c r="F23"/>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="13">
-        <v>57.5</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="C24" s="13">
-        <v>1</v>
-      </c>
-      <c r="D24" s="13">
-        <v>1</v>
-      </c>
-      <c r="E24" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="F24" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
+      <c r="A24"/>
+      <c r="D24"/>
+      <c r="E24"/>
+      <c r="F24"/>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="13">
-        <v>60</v>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="C25" s="13">
-        <v>1</v>
-      </c>
-      <c r="D25" s="13">
-        <v>1</v>
-      </c>
-      <c r="E25" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="F25" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
+      <c r="A25"/>
+      <c r="D25"/>
+      <c r="E25"/>
+      <c r="F25"/>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="13">
-        <v>62.5</v>
-      </c>
-      <c r="B26" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="C26" s="13">
-        <v>1</v>
-      </c>
-      <c r="D26" s="13">
-        <v>1</v>
-      </c>
-      <c r="E26" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="F26" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
+      <c r="A26"/>
+      <c r="D26"/>
+      <c r="E26"/>
+      <c r="F26"/>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="13">
-        <v>65</v>
-      </c>
-      <c r="B27" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="C27" s="13">
-        <v>1</v>
-      </c>
-      <c r="D27" s="13">
-        <v>1</v>
-      </c>
-      <c r="E27" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="F27" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
+      <c r="A27"/>
+      <c r="D27"/>
+      <c r="E27"/>
+      <c r="F27"/>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="13">
-        <v>67.5</v>
-      </c>
-      <c r="B28" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="C28" s="13">
-        <v>1</v>
-      </c>
-      <c r="D28" s="13">
-        <v>1</v>
-      </c>
-      <c r="E28" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="F28" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
+      <c r="A28"/>
+      <c r="D28"/>
+      <c r="E28"/>
+      <c r="F28"/>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="13">
-        <v>70</v>
-      </c>
-      <c r="B29" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="C29" s="13">
-        <v>1</v>
-      </c>
-      <c r="D29" s="13">
-        <v>1</v>
-      </c>
-      <c r="E29" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="F29" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
+      <c r="A29"/>
+      <c r="D29"/>
+      <c r="E29"/>
+      <c r="F29"/>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="13">
-        <v>72.5</v>
-      </c>
-      <c r="B30" s="13" t="s">
-        <v>104</v>
-      </c>
-      <c r="C30" s="13">
-        <v>1</v>
-      </c>
-      <c r="D30" s="13">
-        <v>1</v>
-      </c>
-      <c r="E30" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="F30" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
+      <c r="A30"/>
+      <c r="D30"/>
+      <c r="E30"/>
+      <c r="F30"/>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="13">
-        <v>75</v>
-      </c>
-      <c r="B31" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C31" s="13">
-        <v>1</v>
-      </c>
-      <c r="D31" s="13">
-        <v>1</v>
-      </c>
-      <c r="E31" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="F31" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
+      <c r="A31"/>
+      <c r="D31"/>
+      <c r="E31"/>
+      <c r="F31"/>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" s="13">
-        <v>77.5</v>
-      </c>
-      <c r="B32" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="C32" s="13">
-        <v>1</v>
-      </c>
-      <c r="D32" s="13">
-        <v>1</v>
-      </c>
-      <c r="E32" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="F32" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
+      <c r="A32"/>
+      <c r="D32"/>
+      <c r="E32"/>
+      <c r="F32"/>
     </row>
     <row r="33" spans="1:6">
-      <c r="A33" s="13">
-        <v>80</v>
-      </c>
-      <c r="B33" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="C33" s="13">
-        <v>1</v>
-      </c>
-      <c r="D33" s="13">
-        <v>1</v>
-      </c>
-      <c r="E33" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="F33" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
+      <c r="A33"/>
+      <c r="D33"/>
+      <c r="E33"/>
+      <c r="F33"/>
     </row>
     <row r="34" spans="1:6">
-      <c r="A34" s="13">
-        <v>82.5</v>
-      </c>
-      <c r="B34" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="C34" s="13">
-        <v>1</v>
-      </c>
-      <c r="D34" s="13">
-        <v>1</v>
-      </c>
-      <c r="E34" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="F34" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
+      <c r="A34"/>
+      <c r="D34"/>
+      <c r="E34"/>
+      <c r="F34"/>
     </row>
     <row r="35" spans="1:6">
-      <c r="A35" s="13">
-        <v>85</v>
-      </c>
-      <c r="B35" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="C35" s="13">
-        <v>1</v>
-      </c>
-      <c r="D35" s="13">
-        <v>1</v>
-      </c>
-      <c r="E35" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="F35" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
+      <c r="A35"/>
+      <c r="D35"/>
+      <c r="E35"/>
+      <c r="F35"/>
     </row>
     <row r="36" spans="1:6">
-      <c r="A36" s="13">
-        <v>87.5</v>
-      </c>
-      <c r="B36" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="C36" s="13">
-        <v>1</v>
-      </c>
-      <c r="D36" s="13">
-        <v>1</v>
-      </c>
-      <c r="E36" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="F36" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
+      <c r="A36"/>
+      <c r="D36"/>
+      <c r="E36"/>
+      <c r="F36"/>
     </row>
     <row r="37" spans="1:6">
-      <c r="A37" s="13">
-        <v>90</v>
-      </c>
-      <c r="B37" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="C37" s="13">
-        <v>1</v>
-      </c>
-      <c r="D37" s="13">
-        <v>1</v>
-      </c>
-      <c r="E37" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="F37" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
+      <c r="A37"/>
+      <c r="D37"/>
+      <c r="E37"/>
+      <c r="F37"/>
     </row>
     <row r="38" spans="1:6">
-      <c r="A38" s="13">
-        <v>92.5</v>
-      </c>
-      <c r="B38" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="C38" s="13">
-        <v>1</v>
-      </c>
-      <c r="D38" s="13">
-        <v>1</v>
-      </c>
-      <c r="E38" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="F38" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
+      <c r="A38"/>
+      <c r="D38"/>
+      <c r="E38"/>
+      <c r="F38"/>
     </row>
     <row r="39" spans="1:6">
-      <c r="A39" s="13">
-        <v>95</v>
-      </c>
-      <c r="B39" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="C39" s="13">
-        <v>1</v>
-      </c>
-      <c r="D39" s="13">
-        <v>1</v>
-      </c>
-      <c r="E39" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="F39" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
+      <c r="A39"/>
+      <c r="D39"/>
+      <c r="E39"/>
+      <c r="F39"/>
     </row>
     <row r="40" spans="1:6">
-      <c r="A40" s="13">
-        <v>97.5</v>
-      </c>
-      <c r="B40" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="C40" s="13">
-        <v>1</v>
-      </c>
-      <c r="D40" s="13">
-        <v>1</v>
-      </c>
-      <c r="E40" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="F40" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
+      <c r="A40"/>
+      <c r="D40"/>
+      <c r="E40"/>
+      <c r="F40"/>
     </row>
     <row r="41" spans="1:6">
-      <c r="A41" s="13">
-        <v>100</v>
-      </c>
-      <c r="B41" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="C41" s="13">
-        <v>1</v>
-      </c>
-      <c r="D41" s="13">
-        <v>1</v>
-      </c>
-      <c r="E41" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="F41" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
+      <c r="A41"/>
+      <c r="D41"/>
+      <c r="E41"/>
+      <c r="F41"/>
     </row>
     <row r="42" spans="1:6">
-      <c r="A42" s="13">
-        <v>102.5</v>
-      </c>
-      <c r="B42" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="C42" s="13">
-        <v>1</v>
-      </c>
-      <c r="D42" s="13">
-        <v>1</v>
-      </c>
-      <c r="E42" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="F42" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
+      <c r="A42"/>
+      <c r="D42"/>
+      <c r="E42"/>
+      <c r="F42"/>
     </row>
     <row r="43" spans="1:6">
-      <c r="A43" s="13">
-        <v>105</v>
-      </c>
-      <c r="B43" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="C43" s="13">
-        <v>1</v>
-      </c>
-      <c r="D43" s="13">
-        <v>1</v>
-      </c>
-      <c r="E43" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="F43" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
+      <c r="A43"/>
+      <c r="D43"/>
+      <c r="E43"/>
+      <c r="F43"/>
     </row>
     <row r="44" spans="1:6">
-      <c r="A44" s="13">
-        <v>107.5</v>
-      </c>
-      <c r="B44" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="C44" s="13">
-        <v>1</v>
-      </c>
-      <c r="D44" s="13">
-        <v>1</v>
-      </c>
-      <c r="E44" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="F44" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
+      <c r="A44"/>
+      <c r="D44"/>
+      <c r="E44"/>
+      <c r="F44"/>
     </row>
     <row r="45" spans="1:6">
-      <c r="A45" s="13">
-        <v>110</v>
-      </c>
-      <c r="B45" s="13" t="s">
-        <v>116</v>
-      </c>
-      <c r="C45" s="13">
-        <v>1</v>
-      </c>
-      <c r="D45" s="13">
-        <v>1</v>
-      </c>
-      <c r="E45" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="F45" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
+      <c r="A45"/>
+      <c r="D45"/>
+      <c r="E45"/>
+      <c r="F45"/>
     </row>
     <row r="46" spans="1:6">
-      <c r="A46" s="13">
-        <v>112.5</v>
-      </c>
-      <c r="B46" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="C46" s="13">
-        <v>1</v>
-      </c>
-      <c r="D46" s="13">
-        <v>1</v>
-      </c>
-      <c r="E46" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="F46" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
+      <c r="A46"/>
+      <c r="D46"/>
+      <c r="E46"/>
+      <c r="F46"/>
     </row>
     <row r="47" spans="1:6">
-      <c r="A47" s="13">
-        <v>115</v>
-      </c>
-      <c r="B47" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="C47" s="13">
-        <v>1</v>
-      </c>
-      <c r="D47" s="13">
-        <v>1</v>
-      </c>
-      <c r="E47" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="F47" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
+      <c r="A47"/>
+      <c r="D47"/>
+      <c r="E47"/>
+      <c r="F47"/>
     </row>
     <row r="48" spans="1:6">
-      <c r="A48" s="13">
-        <v>117.5</v>
-      </c>
-      <c r="B48" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="C48" s="13">
-        <v>1</v>
-      </c>
-      <c r="D48" s="13">
-        <v>1</v>
-      </c>
-      <c r="E48" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="F48" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
+      <c r="A48"/>
+      <c r="D48"/>
+      <c r="E48"/>
+      <c r="F48"/>
     </row>
     <row r="49" spans="1:6">
-      <c r="A49" s="13">
-        <v>120</v>
-      </c>
-      <c r="B49" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="C49" s="13">
-        <v>1</v>
-      </c>
-      <c r="D49" s="13">
-        <v>1</v>
-      </c>
-      <c r="E49" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="F49" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
+      <c r="A49"/>
+      <c r="D49"/>
+      <c r="E49"/>
+      <c r="F49"/>
     </row>
     <row r="50" spans="1:6">
-      <c r="A50" s="13">
-        <v>122.5</v>
-      </c>
-      <c r="B50" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="C50" s="13">
-        <v>1</v>
-      </c>
-      <c r="D50" s="13">
-        <v>1</v>
-      </c>
-      <c r="E50" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="F50" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
+      <c r="A50"/>
+      <c r="D50"/>
+      <c r="E50"/>
+      <c r="F50"/>
     </row>
     <row r="51" spans="1:6">
-      <c r="A51" s="13">
-        <v>125</v>
-      </c>
-      <c r="B51" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="C51" s="13">
-        <v>1</v>
-      </c>
-      <c r="D51" s="13">
-        <v>1</v>
-      </c>
-      <c r="E51" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="F51" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
+      <c r="A51"/>
+      <c r="D51"/>
+      <c r="E51"/>
+      <c r="F51"/>
     </row>
     <row r="52" spans="1:6">
-      <c r="A52" s="13">
-        <v>127.5</v>
-      </c>
-      <c r="B52" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="C52" s="13">
-        <v>0.1</v>
-      </c>
-      <c r="D52" s="13">
-        <v>0.1</v>
-      </c>
-      <c r="E52" s="13">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="F52" s="13">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
+      <c r="A52"/>
+      <c r="D52"/>
+      <c r="E52"/>
+      <c r="F52"/>
     </row>
     <row r="53" spans="1:6">
-      <c r="A53" s="13">
-        <v>130</v>
-      </c>
-      <c r="B53" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="C53" s="13">
-        <v>0.1</v>
-      </c>
-      <c r="D53" s="13">
-        <v>0.1</v>
-      </c>
-      <c r="E53" s="13">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="F53" s="13">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
+      <c r="A53"/>
+      <c r="D53"/>
+      <c r="E53"/>
+      <c r="F53"/>
     </row>
     <row r="54" spans="1:6">
-      <c r="A54" s="13">
-        <v>132.5</v>
-      </c>
-      <c r="B54" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="C54" s="13">
-        <v>0.1</v>
-      </c>
-      <c r="D54" s="13">
-        <v>0.1</v>
-      </c>
-      <c r="E54" s="13">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="F54" s="13">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
+      <c r="A54"/>
+      <c r="D54"/>
+      <c r="E54"/>
+      <c r="F54"/>
     </row>
     <row r="55" spans="1:6">
-      <c r="A55" s="13">
-        <v>135</v>
-      </c>
-      <c r="B55" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="C55" s="13">
-        <v>0.1</v>
-      </c>
-      <c r="D55" s="13">
-        <v>0.1</v>
-      </c>
-      <c r="E55" s="13">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="F55" s="13">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
+      <c r="A55"/>
+      <c r="D55"/>
+      <c r="E55"/>
+      <c r="F55"/>
     </row>
     <row r="56" spans="1:6">
-      <c r="A56" s="13">
-        <v>137.5</v>
-      </c>
-      <c r="B56" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="C56" s="13">
-        <v>0.1</v>
-      </c>
-      <c r="D56" s="13">
-        <v>0.1</v>
-      </c>
-      <c r="E56" s="13">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="F56" s="13">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
+      <c r="A56"/>
+      <c r="D56"/>
+      <c r="E56"/>
+      <c r="F56"/>
     </row>
     <row r="57" spans="1:6">
-      <c r="A57" s="13">
-        <v>140</v>
-      </c>
-      <c r="B57" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="C57" s="13">
-        <v>0.1</v>
-      </c>
-      <c r="D57" s="13">
-        <v>0.1</v>
-      </c>
-      <c r="E57" s="13">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="F57" s="13">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
+      <c r="A57"/>
+      <c r="D57"/>
+      <c r="E57"/>
+      <c r="F57"/>
     </row>
     <row r="58" spans="1:6">
-      <c r="A58" s="13">
-        <v>142.5</v>
-      </c>
-      <c r="B58" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="C58" s="13">
-        <v>0.1</v>
-      </c>
-      <c r="D58" s="13">
-        <v>0.1</v>
-      </c>
-      <c r="E58" s="13">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="F58" s="13">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
+      <c r="A58"/>
+      <c r="D58"/>
+      <c r="E58"/>
+      <c r="F58"/>
     </row>
     <row r="59" spans="1:6">
-      <c r="A59" s="13">
-        <v>145</v>
-      </c>
-      <c r="B59" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="C59" s="13">
-        <v>1</v>
-      </c>
-      <c r="D59" s="13">
-        <v>1</v>
-      </c>
-      <c r="E59" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="F59" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
+      <c r="A59"/>
+      <c r="D59"/>
+      <c r="E59"/>
+      <c r="F59"/>
     </row>
     <row r="60" spans="1:6">
-      <c r="A60" s="13">
-        <v>147.5</v>
-      </c>
-      <c r="B60" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="C60" s="13">
-        <v>1</v>
-      </c>
-      <c r="D60" s="13">
-        <v>1</v>
-      </c>
-      <c r="E60" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="F60" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
+      <c r="A60"/>
+      <c r="D60"/>
+      <c r="E60"/>
+      <c r="F60"/>
     </row>
     <row r="61" spans="1:6">
-      <c r="A61" s="13">
-        <v>150</v>
-      </c>
-      <c r="B61" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="C61" s="13">
-        <v>1</v>
-      </c>
-      <c r="D61" s="13">
-        <v>1</v>
-      </c>
-      <c r="E61" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="F61" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
+      <c r="A61"/>
+      <c r="D61"/>
+      <c r="E61"/>
+      <c r="F61"/>
     </row>
     <row r="62" spans="1:6">
-      <c r="A62" s="13">
-        <v>152.5</v>
-      </c>
-      <c r="B62" s="13" t="s">
-        <v>129</v>
-      </c>
-      <c r="C62" s="13">
-        <v>1</v>
-      </c>
-      <c r="D62" s="13">
-        <v>1</v>
-      </c>
-      <c r="E62" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="F62" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
+      <c r="A62"/>
+      <c r="D62"/>
+      <c r="E62"/>
+      <c r="F62"/>
     </row>
     <row r="63" spans="1:6">
-      <c r="A63" s="13">
-        <v>155</v>
-      </c>
-      <c r="B63" s="13" t="s">
-        <v>130</v>
-      </c>
-      <c r="C63" s="13">
-        <v>1</v>
-      </c>
-      <c r="D63" s="13">
-        <v>1</v>
-      </c>
-      <c r="E63" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="F63" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
+      <c r="A63"/>
+      <c r="D63"/>
+      <c r="E63"/>
+      <c r="F63"/>
     </row>
     <row r="64" spans="1:6">
-      <c r="A64" s="13">
-        <v>157.5</v>
-      </c>
-      <c r="B64" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="C64" s="13">
-        <v>1</v>
-      </c>
-      <c r="D64" s="13">
-        <v>1</v>
-      </c>
-      <c r="E64" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="F64" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
+      <c r="A64"/>
+      <c r="D64"/>
+      <c r="E64"/>
+      <c r="F64"/>
     </row>
     <row r="65" spans="1:6">
-      <c r="A65" s="13">
-        <v>160</v>
-      </c>
-      <c r="B65" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="C65" s="13">
-        <v>1</v>
-      </c>
-      <c r="D65" s="13">
-        <v>1</v>
-      </c>
-      <c r="E65" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="F65" s="13">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
+      <c r="A65"/>
+      <c r="D65"/>
+      <c r="E65"/>
+      <c r="F65"/>
     </row>
     <row r="66" spans="1:6">
-      <c r="A66" s="13">
-        <v>162.5</v>
-      </c>
-      <c r="B66" s="13" t="s">
-        <v>104</v>
-      </c>
-      <c r="C66" s="13">
-        <v>1</v>
-      </c>
-      <c r="D66" s="13">
-        <v>1</v>
-      </c>
-      <c r="E66" s="13">
-        <f t="shared" ref="E66:F91" si="1">C66*1000</f>
-        <v>1000</v>
-      </c>
-      <c r="F66" s="13">
-        <f t="shared" si="1"/>
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6">
-      <c r="A67" s="13">
-        <v>165</v>
-      </c>
-      <c r="B67" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C67" s="13">
-        <v>1</v>
-      </c>
-      <c r="D67" s="13">
-        <v>1</v>
-      </c>
-      <c r="E67" s="13">
-        <f t="shared" si="1"/>
-        <v>1000</v>
-      </c>
-      <c r="F67" s="13">
-        <f t="shared" si="1"/>
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6">
-      <c r="A68" s="13">
-        <v>167.5</v>
-      </c>
-      <c r="B68" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="C68" s="13">
-        <v>1</v>
-      </c>
-      <c r="D68" s="13">
-        <v>1</v>
-      </c>
-      <c r="E68" s="13">
-        <f t="shared" si="1"/>
-        <v>1000</v>
-      </c>
-      <c r="F68" s="13">
-        <f t="shared" si="1"/>
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6">
-      <c r="A69" s="13">
-        <v>170</v>
-      </c>
-      <c r="B69" s="13" t="s">
-        <v>133</v>
-      </c>
-      <c r="C69" s="13">
-        <v>1</v>
-      </c>
-      <c r="D69" s="13">
-        <v>1</v>
-      </c>
-      <c r="E69" s="13">
-        <f t="shared" si="1"/>
-        <v>1000</v>
-      </c>
-      <c r="F69" s="13">
-        <f t="shared" si="1"/>
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6">
-      <c r="A70" s="13">
-        <v>172.5</v>
-      </c>
-      <c r="B70" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="C70" s="13">
-        <v>1</v>
-      </c>
-      <c r="D70" s="13">
-        <v>1</v>
-      </c>
-      <c r="E70" s="13">
-        <f t="shared" si="1"/>
-        <v>1000</v>
-      </c>
-      <c r="F70" s="13">
-        <f t="shared" si="1"/>
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6">
-      <c r="A71" s="13">
-        <v>175</v>
-      </c>
-      <c r="B71" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="C71" s="13">
-        <v>1</v>
-      </c>
-      <c r="D71" s="13">
-        <v>1</v>
-      </c>
-      <c r="E71" s="13">
-        <f t="shared" si="1"/>
-        <v>1000</v>
-      </c>
-      <c r="F71" s="13">
-        <f t="shared" si="1"/>
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6">
-      <c r="A72" s="13">
-        <v>177.5</v>
-      </c>
-      <c r="B72" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="C72" s="13">
-        <v>1</v>
-      </c>
-      <c r="D72" s="13">
-        <v>1</v>
-      </c>
-      <c r="E72" s="13">
-        <f t="shared" si="1"/>
-        <v>1000</v>
-      </c>
-      <c r="F72" s="13">
-        <f t="shared" si="1"/>
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6">
-      <c r="A73" s="13">
-        <v>180</v>
-      </c>
-      <c r="B73" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="C73" s="13">
-        <v>1</v>
-      </c>
-      <c r="D73" s="13">
-        <v>1</v>
-      </c>
-      <c r="E73" s="13">
-        <f t="shared" si="1"/>
-        <v>1000</v>
-      </c>
-      <c r="F73" s="13">
-        <f t="shared" si="1"/>
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6">
-      <c r="A74" s="13">
-        <v>182.5</v>
-      </c>
-      <c r="B74" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="C74" s="13">
-        <v>1</v>
-      </c>
-      <c r="D74" s="13">
-        <v>1</v>
-      </c>
-      <c r="E74" s="13">
-        <f t="shared" si="1"/>
-        <v>1000</v>
-      </c>
-      <c r="F74" s="13">
-        <f t="shared" si="1"/>
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6">
-      <c r="A75" s="13">
-        <v>185</v>
-      </c>
-      <c r="B75" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="C75" s="13">
-        <v>1</v>
-      </c>
-      <c r="D75" s="13">
-        <v>1</v>
-      </c>
-      <c r="E75" s="13">
-        <f t="shared" si="1"/>
-        <v>1000</v>
-      </c>
-      <c r="F75" s="13">
-        <f t="shared" si="1"/>
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6">
-      <c r="A76" s="13">
-        <v>187.5</v>
-      </c>
-      <c r="B76" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="C76" s="13">
-        <v>1</v>
-      </c>
-      <c r="D76" s="13">
-        <v>1</v>
-      </c>
-      <c r="E76" s="13">
-        <f t="shared" si="1"/>
-        <v>1000</v>
-      </c>
-      <c r="F76" s="13">
-        <f t="shared" si="1"/>
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6">
-      <c r="A77" s="13">
-        <v>190</v>
-      </c>
-      <c r="B77" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="C77" s="13">
-        <v>1</v>
-      </c>
-      <c r="D77" s="13">
-        <v>1</v>
-      </c>
-      <c r="E77" s="13">
-        <f t="shared" si="1"/>
-        <v>1000</v>
-      </c>
-      <c r="F77" s="13">
-        <f t="shared" si="1"/>
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6">
-      <c r="A78" s="13">
-        <v>192.5</v>
-      </c>
-      <c r="B78" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="C78" s="13">
-        <v>1</v>
-      </c>
-      <c r="D78" s="13">
-        <v>1</v>
-      </c>
-      <c r="E78" s="13">
-        <f t="shared" si="1"/>
-        <v>1000</v>
-      </c>
-      <c r="F78" s="13">
-        <f t="shared" si="1"/>
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6">
-      <c r="A79" s="13">
-        <v>195</v>
-      </c>
-      <c r="B79" s="13" t="s">
-        <v>136</v>
-      </c>
-      <c r="C79" s="13">
-        <v>1</v>
-      </c>
-      <c r="D79" s="13">
-        <v>1</v>
-      </c>
-      <c r="E79" s="13">
-        <f t="shared" si="1"/>
-        <v>1000</v>
-      </c>
-      <c r="F79" s="13">
-        <f t="shared" si="1"/>
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6">
-      <c r="A80" s="13">
-        <v>197.5</v>
-      </c>
-      <c r="B80" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="C80" s="13">
-        <v>1</v>
-      </c>
-      <c r="D80" s="13">
-        <v>1</v>
-      </c>
-      <c r="E80" s="13">
-        <f t="shared" si="1"/>
-        <v>1000</v>
-      </c>
-      <c r="F80" s="13">
-        <f t="shared" si="1"/>
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6">
-      <c r="A81" s="13">
-        <v>200</v>
-      </c>
-      <c r="B81" s="13" t="s">
-        <v>116</v>
-      </c>
-      <c r="C81" s="13">
-        <v>1</v>
-      </c>
-      <c r="D81" s="13">
-        <v>1</v>
-      </c>
-      <c r="E81" s="13">
-        <f t="shared" si="1"/>
-        <v>1000</v>
-      </c>
-      <c r="F81" s="13">
-        <f t="shared" si="1"/>
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6">
-      <c r="A82" s="13">
-        <v>202.5</v>
-      </c>
-      <c r="B82" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="C82" s="13">
-        <v>1</v>
-      </c>
-      <c r="D82" s="13">
-        <v>1</v>
-      </c>
-      <c r="E82" s="13">
-        <f t="shared" si="1"/>
-        <v>1000</v>
-      </c>
-      <c r="F82" s="13">
-        <f t="shared" si="1"/>
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6">
-      <c r="A83" s="13">
-        <v>205</v>
-      </c>
-      <c r="B83" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="C83" s="13">
-        <v>1</v>
-      </c>
-      <c r="D83" s="13">
-        <v>1</v>
-      </c>
-      <c r="E83" s="13">
-        <f t="shared" si="1"/>
-        <v>1000</v>
-      </c>
-      <c r="F83" s="13">
-        <f t="shared" si="1"/>
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6">
-      <c r="A84" s="13">
-        <v>207.5</v>
-      </c>
-      <c r="B84" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="C84" s="13">
-        <v>1</v>
-      </c>
-      <c r="D84" s="13">
-        <v>1</v>
-      </c>
-      <c r="E84" s="13">
-        <f t="shared" si="1"/>
-        <v>1000</v>
-      </c>
-      <c r="F84" s="13">
-        <f t="shared" si="1"/>
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6">
-      <c r="A85" s="13">
-        <v>210</v>
-      </c>
-      <c r="B85" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="C85" s="13">
-        <v>1</v>
-      </c>
-      <c r="D85" s="13">
-        <v>1</v>
-      </c>
-      <c r="E85" s="13">
-        <f t="shared" si="1"/>
-        <v>1000</v>
-      </c>
-      <c r="F85" s="13">
-        <f t="shared" si="1"/>
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6">
-      <c r="A86" s="13">
-        <v>212.5</v>
-      </c>
-      <c r="B86" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="C86" s="13">
-        <v>1</v>
-      </c>
-      <c r="D86" s="13">
-        <v>1</v>
-      </c>
-      <c r="E86" s="13">
-        <f t="shared" si="1"/>
-        <v>1000</v>
-      </c>
-      <c r="F86" s="13">
-        <f t="shared" si="1"/>
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6">
-      <c r="A87" s="13">
-        <v>215</v>
-      </c>
-      <c r="B87" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="C87" s="13">
-        <v>1</v>
-      </c>
-      <c r="D87" s="13">
-        <v>1</v>
-      </c>
-      <c r="E87" s="13">
-        <f t="shared" si="1"/>
-        <v>1000</v>
-      </c>
-      <c r="F87" s="13">
-        <f t="shared" si="1"/>
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6">
-      <c r="A88" s="13">
-        <v>217.5</v>
-      </c>
-      <c r="B88" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="C88" s="13">
-        <v>0.1</v>
-      </c>
-      <c r="D88" s="13">
-        <v>0.1</v>
-      </c>
-      <c r="E88" s="13">
-        <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
-      <c r="F88" s="13">
-        <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6">
-      <c r="A89" s="13">
-        <v>220</v>
-      </c>
-      <c r="B89" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="C89" s="13">
-        <v>0.1</v>
-      </c>
-      <c r="D89" s="13">
-        <v>0.1</v>
-      </c>
-      <c r="E89" s="13">
-        <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
-      <c r="F89" s="13">
-        <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6">
-      <c r="A90" s="13">
-        <v>222.5</v>
-      </c>
-      <c r="B90" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="C90" s="13">
-        <v>0.1</v>
-      </c>
-      <c r="D90" s="13">
-        <v>0.1</v>
-      </c>
-      <c r="E90" s="13">
-        <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
-      <c r="F90" s="13">
-        <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6">
-      <c r="A91" s="13">
-        <v>225</v>
-      </c>
-      <c r="B91" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="C91" s="13">
-        <v>0.1</v>
-      </c>
-      <c r="D91" s="13">
-        <v>0.1</v>
-      </c>
-      <c r="E91" s="13">
-        <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
-      <c r="F91" s="13">
-        <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
+      <c r="A66"/>
+      <c r="D66"/>
+      <c r="E66"/>
+      <c r="F66"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Analysis A245: Dependency of second harmonic power on incoming beam polarization.
</commit_message>
<xml_diff>
--- a/245/data/Super_awesome_optical_freq_doubling.xlsx
+++ b/245/data/Super_awesome_optical_freq_doubling.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="19035" windowHeight="8445" activeTab="7"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="19035" windowHeight="8445" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -325,7 +325,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -340,7 +340,6 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -8298,7 +8297,7 @@
   <dimension ref="A1:G81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="A5" sqref="A5:G81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -10270,8 +10269,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -10504,680 +10503,1097 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F66"/>
+  <dimension ref="A1:D77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="11.42578125" style="13"/>
-    <col min="5" max="6" width="11.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="13"/>
+    <col min="3" max="3" width="11.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1">
+    <row r="1" spans="1:4">
+      <c r="A1" s="13">
         <v>0</v>
       </c>
       <c r="B1" s="13">
-        <v>112.553</v>
-      </c>
-      <c r="C1" s="13">
-        <v>0.37819999999999998</v>
+        <v>32</v>
+      </c>
+      <c r="C1">
+        <v>0.2</v>
       </c>
       <c r="D1">
-        <v>23.7</v>
-      </c>
-      <c r="E1">
-        <v>0.01</v>
-      </c>
-      <c r="F1">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="13">
         <v>2.5</v>
       </c>
       <c r="B2" s="13">
-        <v>111.693987190893</v>
-      </c>
-      <c r="C2" s="13">
-        <v>0.78148028788541435</v>
+        <v>28.5</v>
+      </c>
+      <c r="C2">
+        <v>0.2</v>
       </c>
       <c r="D2">
-        <v>23</v>
-      </c>
-      <c r="E2">
-        <v>0.01</v>
-      </c>
-      <c r="F2">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="13">
         <v>5</v>
       </c>
-      <c r="B3" s="14">
-        <v>109.1431729603935</v>
-      </c>
-      <c r="C3" s="14">
-        <v>1.3989182962915241</v>
+      <c r="B3" s="13">
+        <v>27.1</v>
+      </c>
+      <c r="C3">
+        <v>0.2</v>
       </c>
       <c r="D3">
-        <v>21.4</v>
-      </c>
-      <c r="E3">
-        <v>0.01</v>
-      </c>
-      <c r="F3">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="13">
         <v>7.5</v>
       </c>
-      <c r="B4" s="14">
-        <v>104.9784293189374</v>
-      </c>
-      <c r="C4" s="14">
-        <v>2.0045938492086832</v>
+      <c r="B4" s="13">
+        <v>24.8</v>
+      </c>
+      <c r="C4">
+        <v>0.2</v>
       </c>
       <c r="D4">
-        <v>19.600000000000001</v>
-      </c>
-      <c r="E4">
-        <v>0.01</v>
-      </c>
-      <c r="F4">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="13">
         <v>10</v>
       </c>
-      <c r="B5" s="14">
-        <v>99.32689879083452</v>
-      </c>
-      <c r="C5" s="14">
-        <v>2.5582646947136163</v>
+      <c r="B5" s="13">
+        <v>22</v>
+      </c>
+      <c r="C5">
+        <v>0.2</v>
       </c>
       <c r="D5">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="13">
+        <v>12.5</v>
+      </c>
+      <c r="B6" s="13">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="C6">
+        <v>0.2</v>
+      </c>
+      <c r="D6">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="13">
+        <v>15</v>
+      </c>
+      <c r="B7" s="13">
+        <v>15.7</v>
+      </c>
+      <c r="C7">
+        <v>0.2</v>
+      </c>
+      <c r="D7">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="13">
         <v>17.5</v>
       </c>
-      <c r="E5">
-        <v>0.01</v>
-      </c>
-      <c r="F5">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6">
-        <v>12.5</v>
-      </c>
-      <c r="B6" s="14">
-        <v>92.361112969723337</v>
-      </c>
-      <c r="C6" s="14">
-        <v>3.037954364508034</v>
-      </c>
-      <c r="D6">
-        <v>15.3</v>
-      </c>
-      <c r="E6">
-        <v>0.01</v>
-      </c>
-      <c r="F6">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7">
-        <v>15</v>
-      </c>
-      <c r="B7" s="14">
-        <v>84.293725423108256</v>
-      </c>
-      <c r="C7" s="14">
-        <v>3.4271936217363717</v>
-      </c>
-      <c r="D7">
+      <c r="B8" s="13">
         <v>12.6</v>
       </c>
-      <c r="E7">
-        <v>0.01</v>
-      </c>
-      <c r="F7">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8">
-        <v>17.5</v>
-      </c>
-      <c r="B8" s="14">
-        <v>75.371019741424803</v>
-      </c>
-      <c r="C8" s="14">
-        <v>3.7132629587734853</v>
+      <c r="C8">
+        <v>0.2</v>
       </c>
       <c r="D8">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="13">
+        <v>20</v>
+      </c>
+      <c r="B9" s="13">
         <v>9.9</v>
       </c>
-      <c r="E8">
-        <v>0.01</v>
-      </c>
-      <c r="F8">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9">
-        <v>20</v>
-      </c>
-      <c r="B9" s="14">
-        <v>65.865390919829281</v>
-      </c>
-      <c r="C9" s="14">
-        <v>3.8869796423982366</v>
+      <c r="C9">
+        <v>0.2</v>
       </c>
       <c r="D9">
-        <v>7</v>
-      </c>
-      <c r="E9">
-        <v>0.01</v>
-      </c>
-      <c r="F9">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="13">
         <v>22.5</v>
       </c>
-      <c r="B10" s="14">
-        <v>56.067029603310949</v>
-      </c>
-      <c r="C10" s="14">
-        <v>3.9427695282759787</v>
+      <c r="B10" s="13">
+        <v>7.7</v>
+      </c>
+      <c r="C10">
+        <v>0.2</v>
       </c>
       <c r="D10">
-        <v>5.2</v>
-      </c>
-      <c r="E10">
-        <v>0.01</v>
-      </c>
-      <c r="F10">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="13">
         <v>25</v>
       </c>
-      <c r="B11" s="14">
-        <v>46.27506306094822</v>
-      </c>
-      <c r="C11" s="14">
-        <v>3.8787510651947663</v>
+      <c r="B11" s="13">
+        <v>5.6</v>
+      </c>
+      <c r="C11">
+        <v>0.2</v>
       </c>
       <c r="D11">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="13">
+        <v>27.5</v>
+      </c>
+      <c r="B12" s="13">
+        <v>4.3</v>
+      </c>
+      <c r="C12">
+        <v>0.2</v>
+      </c>
+      <c r="D12">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="13">
+        <v>30</v>
+      </c>
+      <c r="B13" s="13">
+        <v>3.2</v>
+      </c>
+      <c r="C13">
+        <v>0.2</v>
+      </c>
+      <c r="D13">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="13">
+        <v>32.5</v>
+      </c>
+      <c r="B14" s="13">
+        <v>2.4</v>
+      </c>
+      <c r="C14">
+        <v>0.2</v>
+      </c>
+      <c r="D14">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="13">
+        <v>35</v>
+      </c>
+      <c r="B15" s="13">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>0.2</v>
+      </c>
+      <c r="D15">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="13">
+        <v>37.5</v>
+      </c>
+      <c r="B16" s="13">
+        <v>1.8</v>
+      </c>
+      <c r="C16">
+        <v>0.2</v>
+      </c>
+      <c r="D16">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="13">
+        <v>40</v>
+      </c>
+      <c r="B17" s="13">
+        <v>1.8</v>
+      </c>
+      <c r="C17">
+        <v>0.2</v>
+      </c>
+      <c r="D17">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="13">
+        <v>42.5</v>
+      </c>
+      <c r="B18" s="13">
+        <v>1.7</v>
+      </c>
+      <c r="C18">
+        <v>0.2</v>
+      </c>
+      <c r="D18">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="13">
+        <v>45</v>
+      </c>
+      <c r="B19" s="13">
+        <v>1.7</v>
+      </c>
+      <c r="C19">
+        <v>0.2</v>
+      </c>
+      <c r="D19">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="13">
+        <v>47.5</v>
+      </c>
+      <c r="B20" s="13">
+        <v>1.8</v>
+      </c>
+      <c r="C20">
+        <v>0.2</v>
+      </c>
+      <c r="D20">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="13">
+        <v>50</v>
+      </c>
+      <c r="B21" s="13">
+        <v>1.8</v>
+      </c>
+      <c r="C21">
+        <v>0.2</v>
+      </c>
+      <c r="D21">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="13">
+        <v>52.5</v>
+      </c>
+      <c r="B22" s="13">
+        <v>1.9</v>
+      </c>
+      <c r="C22">
+        <v>0.2</v>
+      </c>
+      <c r="D22">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="13">
+        <v>55</v>
+      </c>
+      <c r="B23" s="13">
+        <v>2.1</v>
+      </c>
+      <c r="C23">
+        <v>0.2</v>
+      </c>
+      <c r="D23">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="13">
+        <v>57.5</v>
+      </c>
+      <c r="B24" s="13">
+        <v>2.6</v>
+      </c>
+      <c r="C24">
+        <v>0.2</v>
+      </c>
+      <c r="D24">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="13">
+        <v>60</v>
+      </c>
+      <c r="B25" s="13">
         <v>3.5</v>
       </c>
-      <c r="E11">
-        <v>0.01</v>
-      </c>
-      <c r="F11">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12">
-        <v>27.5</v>
-      </c>
-      <c r="B12" s="14">
-        <v>36.788423340264913</v>
-      </c>
-      <c r="C12" s="14">
-        <v>3.696752369519364</v>
-      </c>
-      <c r="D12">
+      <c r="C25">
+        <v>0.2</v>
+      </c>
+      <c r="D25">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="13">
+        <v>62.5</v>
+      </c>
+      <c r="B26" s="13">
+        <v>4.7</v>
+      </c>
+      <c r="C26">
+        <v>0.2</v>
+      </c>
+      <c r="D26">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="13">
+        <v>65</v>
+      </c>
+      <c r="B27" s="13">
+        <v>6.3</v>
+      </c>
+      <c r="C27">
+        <v>0.2</v>
+      </c>
+      <c r="D27">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="13">
+        <v>67.5</v>
+      </c>
+      <c r="B28" s="13">
+        <v>8.1</v>
+      </c>
+      <c r="C28">
+        <v>0.2</v>
+      </c>
+      <c r="D28">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="13">
+        <v>70</v>
+      </c>
+      <c r="B29" s="13">
+        <v>10.7</v>
+      </c>
+      <c r="C29">
+        <v>0.2</v>
+      </c>
+      <c r="D29">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="13">
+        <v>72.5</v>
+      </c>
+      <c r="B30" s="13">
+        <v>12.6</v>
+      </c>
+      <c r="C30">
+        <v>0.2</v>
+      </c>
+      <c r="D30">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="13">
+        <v>75</v>
+      </c>
+      <c r="B31" s="13">
+        <v>15.7</v>
+      </c>
+      <c r="C31">
+        <v>0.2</v>
+      </c>
+      <c r="D31">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="13">
+        <v>77.5</v>
+      </c>
+      <c r="B32" s="13">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="C32">
+        <v>0.2</v>
+      </c>
+      <c r="D32">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="13">
+        <v>80</v>
+      </c>
+      <c r="B33" s="13">
+        <v>20.6</v>
+      </c>
+      <c r="C33">
+        <v>0.2</v>
+      </c>
+      <c r="D33">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="13">
+        <v>82.5</v>
+      </c>
+      <c r="B34" s="13">
+        <v>22.6</v>
+      </c>
+      <c r="C34">
+        <v>0.2</v>
+      </c>
+      <c r="D34">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="13">
+        <v>85</v>
+      </c>
+      <c r="B35" s="13">
+        <v>23.8</v>
+      </c>
+      <c r="C35">
+        <v>0.2</v>
+      </c>
+      <c r="D35">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="13">
+        <v>87.5</v>
+      </c>
+      <c r="B36" s="13">
+        <v>24.4</v>
+      </c>
+      <c r="C36">
+        <v>0.2</v>
+      </c>
+      <c r="D36">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="13">
+        <v>90</v>
+      </c>
+      <c r="B37" s="13">
+        <v>24.3</v>
+      </c>
+      <c r="C37">
+        <v>0.2</v>
+      </c>
+      <c r="D37">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="13">
+        <v>92.5</v>
+      </c>
+      <c r="B38" s="13">
+        <v>23.6</v>
+      </c>
+      <c r="C38">
+        <v>0.2</v>
+      </c>
+      <c r="D38">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="13">
+        <v>95</v>
+      </c>
+      <c r="B39" s="13">
+        <v>22.3</v>
+      </c>
+      <c r="C39">
+        <v>0.2</v>
+      </c>
+      <c r="D39">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="13">
+        <v>97.5</v>
+      </c>
+      <c r="B40" s="13">
+        <v>20.6</v>
+      </c>
+      <c r="C40">
+        <v>0.2</v>
+      </c>
+      <c r="D40">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="13">
+        <v>100</v>
+      </c>
+      <c r="B41" s="13">
+        <v>18.2</v>
+      </c>
+      <c r="C41">
+        <v>0.2</v>
+      </c>
+      <c r="D41">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="13">
+        <v>102.5</v>
+      </c>
+      <c r="B42" s="13">
+        <v>15.7</v>
+      </c>
+      <c r="C42">
+        <v>0.2</v>
+      </c>
+      <c r="D42">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="13">
+        <v>105</v>
+      </c>
+      <c r="B43" s="13">
+        <v>14.5</v>
+      </c>
+      <c r="C43">
+        <v>0.2</v>
+      </c>
+      <c r="D43">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="13">
+        <v>107.5</v>
+      </c>
+      <c r="B44" s="13">
+        <v>11.2</v>
+      </c>
+      <c r="C44">
+        <v>0.2</v>
+      </c>
+      <c r="D44">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="13">
+        <v>110</v>
+      </c>
+      <c r="B45" s="13">
+        <v>8.5</v>
+      </c>
+      <c r="C45">
+        <v>0.2</v>
+      </c>
+      <c r="D45">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="13">
+        <v>112.5</v>
+      </c>
+      <c r="B46" s="13">
+        <v>6.8</v>
+      </c>
+      <c r="C46">
+        <v>0.2</v>
+      </c>
+      <c r="D46">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="13">
+        <v>115</v>
+      </c>
+      <c r="B47" s="13">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="C47">
+        <v>0.2</v>
+      </c>
+      <c r="D47">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="13">
+        <v>117.5</v>
+      </c>
+      <c r="B48" s="13">
+        <v>3.9</v>
+      </c>
+      <c r="C48">
+        <v>0.2</v>
+      </c>
+      <c r="D48">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="13">
+        <v>120</v>
+      </c>
+      <c r="B49" s="13">
+        <v>2.8</v>
+      </c>
+      <c r="C49">
+        <v>0.2</v>
+      </c>
+      <c r="D49">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="13">
+        <v>122.5</v>
+      </c>
+      <c r="B50" s="13">
         <v>2.2999999999999998</v>
       </c>
-      <c r="E12">
-        <v>0.01</v>
-      </c>
-      <c r="F12">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13">
-        <v>30</v>
-      </c>
-      <c r="B13" s="14">
-        <v>27.896721381367488</v>
-      </c>
-      <c r="C13" s="14">
-        <v>3.4022346269051393</v>
-      </c>
-      <c r="D13">
-        <v>1.3</v>
-      </c>
-      <c r="E13">
-        <v>0.01</v>
-      </c>
-      <c r="F13">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14">
-        <v>32.5</v>
-      </c>
-      <c r="B14" s="14">
-        <v>19.871405688603378</v>
-      </c>
-      <c r="C14" s="14">
-        <v>3.0041138395583999</v>
-      </c>
-      <c r="D14">
-        <v>0.8</v>
-      </c>
-      <c r="E14">
-        <v>0.01</v>
-      </c>
-      <c r="F14">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15">
-        <v>35</v>
-      </c>
-      <c r="B15" s="14">
-        <v>12.957475470424107</v>
-      </c>
-      <c r="C15" s="14">
-        <v>2.5144818402151099</v>
-      </c>
-      <c r="D15">
-        <v>0.4</v>
-      </c>
-      <c r="E15">
-        <v>0.01</v>
-      </c>
-      <c r="F15">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16">
-        <v>37.5</v>
-      </c>
-      <c r="B16" s="14">
-        <v>7.3660012311676759</v>
-      </c>
-      <c r="C16" s="14">
-        <v>1.948232931073471</v>
-      </c>
-      <c r="D16">
-        <v>0.2</v>
-      </c>
-      <c r="E16">
-        <v>0.01</v>
-      </c>
-      <c r="F16">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17">
-        <v>40</v>
-      </c>
-      <c r="B17" s="14">
-        <v>3.2676811483437938</v>
-      </c>
-      <c r="C17" s="14">
-        <v>1.322606436529951</v>
-      </c>
-      <c r="D17">
-        <v>0.11</v>
-      </c>
-      <c r="E17">
-        <v>0.01</v>
-      </c>
-      <c r="F17">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18">
-        <v>42.5</v>
-      </c>
-      <c r="B18" s="13">
-        <v>0.78762994824019816</v>
-      </c>
-      <c r="C18" s="13">
-        <v>0.65665852544455006</v>
-      </c>
-      <c r="D18">
-        <v>0.09</v>
-      </c>
-      <c r="E18">
-        <v>0.01</v>
-      </c>
-      <c r="F18">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19">
-        <v>45</v>
-      </c>
-      <c r="B19" s="13">
-        <v>1.5593665949043955E-3</v>
-      </c>
-      <c r="C19" s="13">
-        <v>2.9320931119283793E-2</v>
-      </c>
-      <c r="D19">
-        <v>0.09</v>
-      </c>
-      <c r="E19">
-        <v>0.01</v>
-      </c>
-      <c r="F19">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20"/>
-      <c r="D20"/>
-      <c r="E20"/>
-      <c r="F20"/>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21"/>
-      <c r="D21"/>
-      <c r="E21"/>
-      <c r="F21"/>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22"/>
-      <c r="D22"/>
-      <c r="E22"/>
-      <c r="F22"/>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23"/>
-      <c r="D23"/>
-      <c r="E23"/>
-      <c r="F23"/>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24"/>
-      <c r="D24"/>
-      <c r="E24"/>
-      <c r="F24"/>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25"/>
-      <c r="D25"/>
-      <c r="E25"/>
-      <c r="F25"/>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26"/>
-      <c r="D26"/>
-      <c r="E26"/>
-      <c r="F26"/>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27"/>
-      <c r="D27"/>
-      <c r="E27"/>
-      <c r="F27"/>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28"/>
-      <c r="D28"/>
-      <c r="E28"/>
-      <c r="F28"/>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29"/>
-      <c r="D29"/>
-      <c r="E29"/>
-      <c r="F29"/>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30"/>
-      <c r="D30"/>
-      <c r="E30"/>
-      <c r="F30"/>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31"/>
-      <c r="D31"/>
-      <c r="E31"/>
-      <c r="F31"/>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32"/>
-      <c r="D32"/>
-      <c r="E32"/>
-      <c r="F32"/>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="A33"/>
-      <c r="D33"/>
-      <c r="E33"/>
-      <c r="F33"/>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34"/>
-      <c r="D34"/>
-      <c r="E34"/>
-      <c r="F34"/>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35"/>
-      <c r="D35"/>
-      <c r="E35"/>
-      <c r="F35"/>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="A36"/>
-      <c r="D36"/>
-      <c r="E36"/>
-      <c r="F36"/>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37"/>
-      <c r="D37"/>
-      <c r="E37"/>
-      <c r="F37"/>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="A38"/>
-      <c r="D38"/>
-      <c r="E38"/>
-      <c r="F38"/>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="A39"/>
-      <c r="D39"/>
-      <c r="E39"/>
-      <c r="F39"/>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40"/>
-      <c r="D40"/>
-      <c r="E40"/>
-      <c r="F40"/>
-    </row>
-    <row r="41" spans="1:6">
-      <c r="A41"/>
-      <c r="D41"/>
-      <c r="E41"/>
-      <c r="F41"/>
-    </row>
-    <row r="42" spans="1:6">
-      <c r="A42"/>
-      <c r="D42"/>
-      <c r="E42"/>
-      <c r="F42"/>
-    </row>
-    <row r="43" spans="1:6">
-      <c r="A43"/>
-      <c r="D43"/>
-      <c r="E43"/>
-      <c r="F43"/>
-    </row>
-    <row r="44" spans="1:6">
-      <c r="A44"/>
-      <c r="D44"/>
-      <c r="E44"/>
-      <c r="F44"/>
-    </row>
-    <row r="45" spans="1:6">
-      <c r="A45"/>
-      <c r="D45"/>
-      <c r="E45"/>
-      <c r="F45"/>
-    </row>
-    <row r="46" spans="1:6">
-      <c r="A46"/>
-      <c r="D46"/>
-      <c r="E46"/>
-      <c r="F46"/>
-    </row>
-    <row r="47" spans="1:6">
-      <c r="A47"/>
-      <c r="D47"/>
-      <c r="E47"/>
-      <c r="F47"/>
-    </row>
-    <row r="48" spans="1:6">
-      <c r="A48"/>
-      <c r="D48"/>
-      <c r="E48"/>
-      <c r="F48"/>
-    </row>
-    <row r="49" spans="1:6">
-      <c r="A49"/>
-      <c r="D49"/>
-      <c r="E49"/>
-      <c r="F49"/>
-    </row>
-    <row r="50" spans="1:6">
-      <c r="A50"/>
-      <c r="D50"/>
-      <c r="E50"/>
-      <c r="F50"/>
-    </row>
-    <row r="51" spans="1:6">
-      <c r="A51"/>
-      <c r="D51"/>
-      <c r="E51"/>
-      <c r="F51"/>
-    </row>
-    <row r="52" spans="1:6">
-      <c r="A52"/>
-      <c r="D52"/>
-      <c r="E52"/>
-      <c r="F52"/>
-    </row>
-    <row r="53" spans="1:6">
-      <c r="A53"/>
-      <c r="D53"/>
-      <c r="E53"/>
-      <c r="F53"/>
-    </row>
-    <row r="54" spans="1:6">
-      <c r="A54"/>
-      <c r="D54"/>
-      <c r="E54"/>
-      <c r="F54"/>
-    </row>
-    <row r="55" spans="1:6">
-      <c r="A55"/>
-      <c r="D55"/>
-      <c r="E55"/>
-      <c r="F55"/>
-    </row>
-    <row r="56" spans="1:6">
-      <c r="A56"/>
-      <c r="D56"/>
-      <c r="E56"/>
-      <c r="F56"/>
-    </row>
-    <row r="57" spans="1:6">
-      <c r="A57"/>
-      <c r="D57"/>
-      <c r="E57"/>
-      <c r="F57"/>
-    </row>
-    <row r="58" spans="1:6">
-      <c r="A58"/>
-      <c r="D58"/>
-      <c r="E58"/>
-      <c r="F58"/>
-    </row>
-    <row r="59" spans="1:6">
-      <c r="A59"/>
-      <c r="D59"/>
-      <c r="E59"/>
-      <c r="F59"/>
-    </row>
-    <row r="60" spans="1:6">
-      <c r="A60"/>
-      <c r="D60"/>
-      <c r="E60"/>
-      <c r="F60"/>
-    </row>
-    <row r="61" spans="1:6">
-      <c r="A61"/>
-      <c r="D61"/>
-      <c r="E61"/>
-      <c r="F61"/>
-    </row>
-    <row r="62" spans="1:6">
-      <c r="A62"/>
-      <c r="D62"/>
-      <c r="E62"/>
-      <c r="F62"/>
-    </row>
-    <row r="63" spans="1:6">
-      <c r="A63"/>
-      <c r="D63"/>
-      <c r="E63"/>
-      <c r="F63"/>
-    </row>
-    <row r="64" spans="1:6">
-      <c r="A64"/>
-      <c r="D64"/>
-      <c r="E64"/>
-      <c r="F64"/>
-    </row>
-    <row r="65" spans="1:6">
-      <c r="A65"/>
-      <c r="D65"/>
-      <c r="E65"/>
-      <c r="F65"/>
-    </row>
-    <row r="66" spans="1:6">
-      <c r="A66"/>
-      <c r="D66"/>
-      <c r="E66"/>
-      <c r="F66"/>
+      <c r="C50">
+        <v>0.2</v>
+      </c>
+      <c r="D50">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="13">
+        <v>125</v>
+      </c>
+      <c r="B51" s="13">
+        <v>1.9</v>
+      </c>
+      <c r="C51">
+        <v>0.2</v>
+      </c>
+      <c r="D51">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="13">
+        <v>127.5</v>
+      </c>
+      <c r="B52" s="13">
+        <v>1.7</v>
+      </c>
+      <c r="C52">
+        <v>0.2</v>
+      </c>
+      <c r="D52">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="13">
+        <v>130</v>
+      </c>
+      <c r="B53" s="13">
+        <v>1.7</v>
+      </c>
+      <c r="C53">
+        <v>0.2</v>
+      </c>
+      <c r="D53">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" s="13">
+        <v>132.5</v>
+      </c>
+      <c r="B54" s="13">
+        <v>1.6</v>
+      </c>
+      <c r="C54">
+        <v>0.2</v>
+      </c>
+      <c r="D54">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="13">
+        <v>135</v>
+      </c>
+      <c r="B55" s="13">
+        <v>1.6</v>
+      </c>
+      <c r="C55">
+        <v>0.2</v>
+      </c>
+      <c r="D55">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="13">
+        <v>137.5</v>
+      </c>
+      <c r="B56" s="13">
+        <v>1.7</v>
+      </c>
+      <c r="C56">
+        <v>0.2</v>
+      </c>
+      <c r="D56">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="13">
+        <v>140</v>
+      </c>
+      <c r="B57" s="13">
+        <v>1.7</v>
+      </c>
+      <c r="C57">
+        <v>0.2</v>
+      </c>
+      <c r="D57">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="13">
+        <v>142.5</v>
+      </c>
+      <c r="B58" s="13">
+        <v>1.8</v>
+      </c>
+      <c r="C58">
+        <v>0.2</v>
+      </c>
+      <c r="D58">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" s="13">
+        <v>145</v>
+      </c>
+      <c r="B59" s="13">
+        <v>2</v>
+      </c>
+      <c r="C59">
+        <v>0.2</v>
+      </c>
+      <c r="D59">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" s="13">
+        <v>147.5</v>
+      </c>
+      <c r="B60" s="13">
+        <v>2.4</v>
+      </c>
+      <c r="C60">
+        <v>0.2</v>
+      </c>
+      <c r="D60">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" s="13">
+        <v>150</v>
+      </c>
+      <c r="B61" s="13">
+        <v>3.4</v>
+      </c>
+      <c r="C61">
+        <v>0.2</v>
+      </c>
+      <c r="D61">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" s="13">
+        <v>152.5</v>
+      </c>
+      <c r="B62" s="13">
+        <v>4.3</v>
+      </c>
+      <c r="C62">
+        <v>0.2</v>
+      </c>
+      <c r="D62">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" s="13">
+        <v>155</v>
+      </c>
+      <c r="B63" s="13">
+        <v>6.1</v>
+      </c>
+      <c r="C63">
+        <v>0.2</v>
+      </c>
+      <c r="D63">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" s="13">
+        <v>157.5</v>
+      </c>
+      <c r="B64" s="13">
+        <v>7.8</v>
+      </c>
+      <c r="C64">
+        <v>0.2</v>
+      </c>
+      <c r="D64">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" s="13">
+        <v>160</v>
+      </c>
+      <c r="B65" s="13">
+        <v>10.3</v>
+      </c>
+      <c r="C65">
+        <v>0.2</v>
+      </c>
+      <c r="D65">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" s="13">
+        <v>162.5</v>
+      </c>
+      <c r="B66" s="13">
+        <v>13</v>
+      </c>
+      <c r="C66">
+        <v>0.2</v>
+      </c>
+      <c r="D66">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" s="13">
+        <v>165</v>
+      </c>
+      <c r="B67" s="13">
+        <v>15.6</v>
+      </c>
+      <c r="C67" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="D67" s="13">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" s="13">
+        <v>167.5</v>
+      </c>
+      <c r="B68" s="13">
+        <v>18</v>
+      </c>
+      <c r="C68" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="D68" s="13">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" s="13">
+        <v>170</v>
+      </c>
+      <c r="B69" s="13">
+        <v>20.9</v>
+      </c>
+      <c r="C69" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="D69" s="13">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" s="13">
+        <v>172.5</v>
+      </c>
+      <c r="B70" s="13">
+        <v>22.6</v>
+      </c>
+      <c r="C70" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="D70" s="13">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" s="13">
+        <v>175</v>
+      </c>
+      <c r="B71" s="13">
+        <v>24.1</v>
+      </c>
+      <c r="C71" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="D71" s="13">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" s="13">
+        <v>177.5</v>
+      </c>
+      <c r="B72" s="13">
+        <v>25.1</v>
+      </c>
+      <c r="C72" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="D72" s="13">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73" s="13">
+        <v>180</v>
+      </c>
+      <c r="B73" s="13">
+        <v>25.4</v>
+      </c>
+      <c r="C73" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="D73" s="13">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" s="13">
+        <v>182.5</v>
+      </c>
+      <c r="B74" s="13">
+        <v>25.1</v>
+      </c>
+      <c r="C74" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="D74" s="13">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75" s="13">
+        <v>185</v>
+      </c>
+      <c r="B75" s="13">
+        <v>23.6</v>
+      </c>
+      <c r="C75" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="D75" s="13">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76" s="13">
+        <v>187.5</v>
+      </c>
+      <c r="B76" s="13">
+        <v>22</v>
+      </c>
+      <c r="C76" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="D76" s="13">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" s="13">
+        <v>190</v>
+      </c>
+      <c r="B77" s="13">
+        <v>19.5</v>
+      </c>
+      <c r="C77" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="D77" s="13">
+        <v>0.1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>